<commit_message>
feat: Added code for creating single-cell samples and added the samples in the design matrix
</commit_message>
<xml_diff>
--- a/DesignMatrix.xlsx
+++ b/DesignMatrix.xlsx
@@ -1,18 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8501C50D-1087-475E-8347-06B3209E4421}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EE43972-9F38-4C8E-8C52-164471863F8F}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="11775" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DesignMatrix" sheetId="2" r:id="rId1"/>
-    <sheet name="Sample info" sheetId="1" r:id="rId2"/>
-    <sheet name="Tissue" sheetId="5" r:id="rId3"/>
-    <sheet name="Labs" sheetId="4" r:id="rId4"/>
-    <sheet name="SubCellType" sheetId="3" r:id="rId5"/>
+    <sheet name="CellTypes" sheetId="6" r:id="rId2"/>
+    <sheet name="Sample info" sheetId="1" r:id="rId3"/>
+    <sheet name="Tissue" sheetId="5" r:id="rId4"/>
+    <sheet name="Labs" sheetId="4" r:id="rId5"/>
+    <sheet name="SubCellType" sheetId="3" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -28,8 +29,26 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>tc={700C9106-279A-4568-A95C-D4F66DD031F0}</author>
+  </authors>
+  <commentList>
+    <comment ref="CY9" authorId="0" shapeId="0" xr:uid="{700C9106-279A-4568-A95C-D4F66DD031F0}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    A bit unclear exactly which type of CD4 memory T cell this is</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="457" uniqueCount="203">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="387" uniqueCount="205">
   <si>
     <t>Sample index</t>
   </si>
@@ -142,12 +161,6 @@
     <t>Sub Cell type</t>
   </si>
   <si>
-    <t>B</t>
-  </si>
-  <si>
-    <t>T</t>
-  </si>
-  <si>
     <t>Poly-A</t>
   </si>
   <si>
@@ -638,13 +651,25 @@
   </si>
   <si>
     <t>130214_SN935_0147_B_D1T9CACXX_AGTCAA_7_read1.fastq.gz, 130214_SN935_0147_B_D1T9CACXX_AGTCAA_7_read2.fastq.gz</t>
+  </si>
+  <si>
+    <t>B cell</t>
+  </si>
+  <si>
+    <t>T cell</t>
+  </si>
+  <si>
+    <t>Single-cell</t>
+  </si>
+  <si>
+    <t>10x pooled single-cell</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -665,6 +690,12 @@
       <color rgb="FF000000"/>
       <name val="Verdana"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="4">
@@ -751,6 +782,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1014,22 +1049,30 @@
 </a:theme>
 </file>
 
+<file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="CY9" dT="2019-08-27T15:46:26.03" personId="{00000000-0000-0000-0000-000000000000}" id="{700C9106-279A-4568-A95C-D4F66DD031F0}">
+    <text>A bit unclear exactly which type of CD4 memory T cell this is</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F369D9C3-2B00-4B3E-B4DE-89D514952C05}">
-  <dimension ref="B2:BX28"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F369D9C3-2B00-4B3E-B4DE-89D514952C05}">
+  <dimension ref="B2:DA28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="AD6" sqref="AD6"/>
+    <sheetView tabSelected="1" topLeftCell="AT1" workbookViewId="0">
+      <selection activeCell="CM16" sqref="CM16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3.85546875" customWidth="1"/>
     <col min="2" max="2" width="18.85546875" customWidth="1"/>
-    <col min="3" max="107" width="3.85546875" customWidth="1"/>
+    <col min="3" max="105" width="3.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:76" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:105" x14ac:dyDescent="0.25">
       <c r="C2" t="s">
         <v>4</v>
       </c>
@@ -1040,13 +1083,16 @@
         <v>4</v>
       </c>
       <c r="AB2" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="BO2" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="3" spans="2:76" x14ac:dyDescent="0.25">
+        <v>183</v>
+      </c>
+      <c r="BY2" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="3" spans="2:105" x14ac:dyDescent="0.25">
       <c r="B3" s="3" t="s">
         <v>29</v>
       </c>
@@ -1272,8 +1318,95 @@
       <c r="BX3" s="3">
         <v>74</v>
       </c>
-    </row>
-    <row r="4" spans="2:76" x14ac:dyDescent="0.25">
+      <c r="BY3" s="3">
+        <v>75</v>
+      </c>
+      <c r="BZ3" s="3">
+        <v>76</v>
+      </c>
+      <c r="CA3" s="3">
+        <v>77</v>
+      </c>
+      <c r="CB3" s="3">
+        <v>78</v>
+      </c>
+      <c r="CC3" s="3">
+        <v>79</v>
+      </c>
+      <c r="CD3" s="3">
+        <v>80</v>
+      </c>
+      <c r="CE3" s="3">
+        <v>81</v>
+      </c>
+      <c r="CF3" s="3">
+        <v>82</v>
+      </c>
+      <c r="CG3" s="3">
+        <v>83</v>
+      </c>
+      <c r="CH3" s="3">
+        <v>84</v>
+      </c>
+      <c r="CI3" s="3">
+        <v>85</v>
+      </c>
+      <c r="CJ3" s="3">
+        <v>86</v>
+      </c>
+      <c r="CK3" s="3">
+        <v>87</v>
+      </c>
+      <c r="CL3" s="3">
+        <v>88</v>
+      </c>
+      <c r="CM3" s="3">
+        <v>89</v>
+      </c>
+      <c r="CN3" s="3">
+        <v>90</v>
+      </c>
+      <c r="CO3" s="3">
+        <v>91</v>
+      </c>
+      <c r="CP3" s="3">
+        <v>92</v>
+      </c>
+      <c r="CQ3" s="3">
+        <v>93</v>
+      </c>
+      <c r="CR3" s="3">
+        <v>94</v>
+      </c>
+      <c r="CS3" s="3">
+        <v>95</v>
+      </c>
+      <c r="CT3" s="3">
+        <v>96</v>
+      </c>
+      <c r="CU3" s="3">
+        <v>97</v>
+      </c>
+      <c r="CV3" s="3">
+        <v>98</v>
+      </c>
+      <c r="CW3" s="3">
+        <v>99</v>
+      </c>
+      <c r="CX3" s="3">
+        <v>100</v>
+      </c>
+      <c r="CY3" s="3">
+        <v>101</v>
+      </c>
+      <c r="CZ3" s="3">
+        <v>102</v>
+      </c>
+      <c r="DA3" s="3">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="4" spans="2:105" x14ac:dyDescent="0.25">
       <c r="B4" s="3" t="s">
         <v>28</v>
       </c>
@@ -1499,8 +1632,95 @@
       <c r="BX4" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="2:76" x14ac:dyDescent="0.25">
+      <c r="BY4" s="4">
+        <v>7</v>
+      </c>
+      <c r="BZ4" s="4">
+        <v>7</v>
+      </c>
+      <c r="CA4" s="4">
+        <v>7</v>
+      </c>
+      <c r="CB4" s="4">
+        <v>7</v>
+      </c>
+      <c r="CC4" s="4">
+        <v>7</v>
+      </c>
+      <c r="CD4" s="4">
+        <v>7</v>
+      </c>
+      <c r="CE4" s="4">
+        <v>7</v>
+      </c>
+      <c r="CF4" s="4">
+        <v>7</v>
+      </c>
+      <c r="CG4" s="4">
+        <v>7</v>
+      </c>
+      <c r="CH4" s="4">
+        <v>7</v>
+      </c>
+      <c r="CI4" s="4">
+        <v>7</v>
+      </c>
+      <c r="CJ4" s="4">
+        <v>7</v>
+      </c>
+      <c r="CK4" s="4">
+        <v>7</v>
+      </c>
+      <c r="CL4" s="4">
+        <v>7</v>
+      </c>
+      <c r="CM4" s="4">
+        <v>7</v>
+      </c>
+      <c r="CN4" s="4">
+        <v>7</v>
+      </c>
+      <c r="CO4" s="4">
+        <v>7</v>
+      </c>
+      <c r="CP4" s="4">
+        <v>7</v>
+      </c>
+      <c r="CQ4" s="4">
+        <v>7</v>
+      </c>
+      <c r="CR4" s="4">
+        <v>7</v>
+      </c>
+      <c r="CS4" s="4">
+        <v>7</v>
+      </c>
+      <c r="CT4" s="4">
+        <v>7</v>
+      </c>
+      <c r="CU4" s="4">
+        <v>7</v>
+      </c>
+      <c r="CV4" s="4">
+        <v>7</v>
+      </c>
+      <c r="CW4" s="4">
+        <v>7</v>
+      </c>
+      <c r="CX4" s="4">
+        <v>7</v>
+      </c>
+      <c r="CY4" s="4">
+        <v>7</v>
+      </c>
+      <c r="CZ4" s="4">
+        <v>7</v>
+      </c>
+      <c r="DA4" s="4">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="2:105" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
         <v>30</v>
       </c>
@@ -1726,8 +1946,95 @@
       <c r="BX5" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="2:76" x14ac:dyDescent="0.25">
+      <c r="BY5" s="4">
+        <v>1</v>
+      </c>
+      <c r="BZ5" s="4">
+        <v>1</v>
+      </c>
+      <c r="CA5" s="4">
+        <v>1</v>
+      </c>
+      <c r="CB5" s="4">
+        <v>1</v>
+      </c>
+      <c r="CC5" s="4">
+        <v>1</v>
+      </c>
+      <c r="CD5" s="4">
+        <v>1</v>
+      </c>
+      <c r="CE5" s="4">
+        <v>1</v>
+      </c>
+      <c r="CF5" s="4">
+        <v>1</v>
+      </c>
+      <c r="CG5" s="4">
+        <v>1</v>
+      </c>
+      <c r="CH5" s="4">
+        <v>1</v>
+      </c>
+      <c r="CI5" s="4">
+        <v>1</v>
+      </c>
+      <c r="CJ5" s="4">
+        <v>1</v>
+      </c>
+      <c r="CK5" s="4">
+        <v>1</v>
+      </c>
+      <c r="CL5" s="4">
+        <v>1</v>
+      </c>
+      <c r="CM5" s="4">
+        <v>1</v>
+      </c>
+      <c r="CN5" s="4">
+        <v>1</v>
+      </c>
+      <c r="CO5" s="4">
+        <v>1</v>
+      </c>
+      <c r="CP5" s="4">
+        <v>1</v>
+      </c>
+      <c r="CQ5" s="4">
+        <v>1</v>
+      </c>
+      <c r="CR5" s="4">
+        <v>1</v>
+      </c>
+      <c r="CS5" s="4">
+        <v>1</v>
+      </c>
+      <c r="CT5" s="4">
+        <v>1</v>
+      </c>
+      <c r="CU5" s="4">
+        <v>1</v>
+      </c>
+      <c r="CV5" s="4">
+        <v>1</v>
+      </c>
+      <c r="CW5" s="4">
+        <v>1</v>
+      </c>
+      <c r="CX5" s="4">
+        <v>1</v>
+      </c>
+      <c r="CY5" s="4">
+        <v>1</v>
+      </c>
+      <c r="CZ5" s="4">
+        <v>1</v>
+      </c>
+      <c r="DA5" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="2:105" x14ac:dyDescent="0.25">
       <c r="B6" s="3" t="s">
         <v>31</v>
       </c>
@@ -1953,8 +2260,95 @@
       <c r="BX6" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="2:76" x14ac:dyDescent="0.25">
+      <c r="BY6" s="4">
+        <v>1</v>
+      </c>
+      <c r="BZ6" s="4">
+        <v>1</v>
+      </c>
+      <c r="CA6" s="4">
+        <v>1</v>
+      </c>
+      <c r="CB6" s="4">
+        <v>1</v>
+      </c>
+      <c r="CC6" s="4">
+        <v>1</v>
+      </c>
+      <c r="CD6" s="4">
+        <v>1</v>
+      </c>
+      <c r="CE6" s="4">
+        <v>1</v>
+      </c>
+      <c r="CF6" s="4">
+        <v>1</v>
+      </c>
+      <c r="CG6" s="4">
+        <v>1</v>
+      </c>
+      <c r="CH6" s="4">
+        <v>1</v>
+      </c>
+      <c r="CI6" s="4">
+        <v>1</v>
+      </c>
+      <c r="CJ6" s="4">
+        <v>1</v>
+      </c>
+      <c r="CK6" s="4">
+        <v>1</v>
+      </c>
+      <c r="CL6" s="4">
+        <v>1</v>
+      </c>
+      <c r="CM6" s="4">
+        <v>1</v>
+      </c>
+      <c r="CN6" s="4">
+        <v>1</v>
+      </c>
+      <c r="CO6" s="4">
+        <v>1</v>
+      </c>
+      <c r="CP6" s="4">
+        <v>1</v>
+      </c>
+      <c r="CQ6" s="4">
+        <v>1</v>
+      </c>
+      <c r="CR6" s="4">
+        <v>1</v>
+      </c>
+      <c r="CS6" s="4">
+        <v>1</v>
+      </c>
+      <c r="CT6" s="4">
+        <v>1</v>
+      </c>
+      <c r="CU6" s="4">
+        <v>1</v>
+      </c>
+      <c r="CV6" s="4">
+        <v>1</v>
+      </c>
+      <c r="CW6" s="4">
+        <v>1</v>
+      </c>
+      <c r="CX6" s="4">
+        <v>1</v>
+      </c>
+      <c r="CY6" s="4">
+        <v>1</v>
+      </c>
+      <c r="CZ6" s="4">
+        <v>1</v>
+      </c>
+      <c r="DA6" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="2:105" x14ac:dyDescent="0.25">
       <c r="B7" s="3" t="s">
         <v>35</v>
       </c>
@@ -2056,10 +2450,39 @@
       <c r="BV7" s="4"/>
       <c r="BW7" s="4"/>
       <c r="BX7" s="4"/>
-    </row>
-    <row r="8" spans="2:76" x14ac:dyDescent="0.25">
+      <c r="BY7" s="4"/>
+      <c r="BZ7" s="4"/>
+      <c r="CA7" s="4"/>
+      <c r="CB7" s="4"/>
+      <c r="CC7" s="4"/>
+      <c r="CD7" s="4"/>
+      <c r="CE7" s="4"/>
+      <c r="CF7" s="4"/>
+      <c r="CG7" s="4"/>
+      <c r="CH7" s="4"/>
+      <c r="CI7" s="4"/>
+      <c r="CJ7" s="4"/>
+      <c r="CK7" s="4"/>
+      <c r="CL7" s="4"/>
+      <c r="CM7" s="4"/>
+      <c r="CN7" s="4"/>
+      <c r="CO7" s="4"/>
+      <c r="CP7" s="4"/>
+      <c r="CQ7" s="4"/>
+      <c r="CR7" s="4"/>
+      <c r="CS7" s="4"/>
+      <c r="CT7" s="4"/>
+      <c r="CU7" s="4"/>
+      <c r="CV7" s="4"/>
+      <c r="CW7" s="4"/>
+      <c r="CX7" s="4"/>
+      <c r="CY7" s="4"/>
+      <c r="CZ7" s="4"/>
+      <c r="DA7" s="4"/>
+    </row>
+    <row r="8" spans="2:105" x14ac:dyDescent="0.25">
       <c r="B8" s="3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C8" s="4">
         <v>2</v>
@@ -2185,8 +2608,37 @@
       <c r="BV8" s="4"/>
       <c r="BW8" s="4"/>
       <c r="BX8" s="4"/>
-    </row>
-    <row r="9" spans="2:76" x14ac:dyDescent="0.25">
+      <c r="BY8" s="4"/>
+      <c r="BZ8" s="4"/>
+      <c r="CA8" s="4"/>
+      <c r="CB8" s="4"/>
+      <c r="CC8" s="4"/>
+      <c r="CD8" s="4"/>
+      <c r="CE8" s="4"/>
+      <c r="CF8" s="4"/>
+      <c r="CG8" s="4"/>
+      <c r="CH8" s="4"/>
+      <c r="CI8" s="4"/>
+      <c r="CJ8" s="4"/>
+      <c r="CK8" s="4"/>
+      <c r="CL8" s="4"/>
+      <c r="CM8" s="4"/>
+      <c r="CN8" s="4"/>
+      <c r="CO8" s="4"/>
+      <c r="CP8" s="4"/>
+      <c r="CQ8" s="4"/>
+      <c r="CR8" s="4"/>
+      <c r="CS8" s="4"/>
+      <c r="CT8" s="4"/>
+      <c r="CU8" s="4"/>
+      <c r="CV8" s="4"/>
+      <c r="CW8" s="4"/>
+      <c r="CX8" s="4"/>
+      <c r="CY8" s="4"/>
+      <c r="CZ8" s="4"/>
+      <c r="DA8" s="4"/>
+    </row>
+    <row r="9" spans="2:105" x14ac:dyDescent="0.25">
       <c r="B9" s="3" t="s">
         <v>36</v>
       </c>
@@ -2412,8 +2864,95 @@
       <c r="BX9" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="2:76" x14ac:dyDescent="0.25">
+      <c r="BY9" s="4">
+        <v>1</v>
+      </c>
+      <c r="BZ9" s="4">
+        <v>1</v>
+      </c>
+      <c r="CA9" s="4">
+        <v>1</v>
+      </c>
+      <c r="CB9" s="4">
+        <v>1</v>
+      </c>
+      <c r="CC9" s="4">
+        <v>1</v>
+      </c>
+      <c r="CD9" s="4">
+        <v>1</v>
+      </c>
+      <c r="CE9" s="4">
+        <v>1</v>
+      </c>
+      <c r="CF9" s="4">
+        <v>1</v>
+      </c>
+      <c r="CG9" s="4">
+        <v>1</v>
+      </c>
+      <c r="CH9" s="4">
+        <v>1</v>
+      </c>
+      <c r="CI9" s="4">
+        <v>1</v>
+      </c>
+      <c r="CJ9" s="4">
+        <v>1</v>
+      </c>
+      <c r="CK9" s="4">
+        <v>1</v>
+      </c>
+      <c r="CL9" s="4">
+        <v>1</v>
+      </c>
+      <c r="CM9" s="4">
+        <v>1</v>
+      </c>
+      <c r="CN9" s="4">
+        <v>1</v>
+      </c>
+      <c r="CO9" s="4">
+        <v>1</v>
+      </c>
+      <c r="CP9" s="4">
+        <v>1</v>
+      </c>
+      <c r="CQ9" s="4">
+        <v>1</v>
+      </c>
+      <c r="CR9" s="4">
+        <v>1</v>
+      </c>
+      <c r="CS9" s="4">
+        <v>1</v>
+      </c>
+      <c r="CT9" s="4">
+        <v>1</v>
+      </c>
+      <c r="CU9" s="4">
+        <v>1</v>
+      </c>
+      <c r="CV9" s="4">
+        <v>1</v>
+      </c>
+      <c r="CW9" s="4">
+        <v>1</v>
+      </c>
+      <c r="CX9" s="4">
+        <v>1</v>
+      </c>
+      <c r="CY9" s="4">
+        <v>10</v>
+      </c>
+      <c r="CZ9" s="4">
+        <v>1</v>
+      </c>
+      <c r="DA9" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="2:105" x14ac:dyDescent="0.25">
       <c r="B10" s="3" t="s">
         <v>32</v>
       </c>
@@ -2639,237 +3178,411 @@
       <c r="BX10" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="2:76" x14ac:dyDescent="0.25">
+      <c r="BY10" s="4">
+        <v>0</v>
+      </c>
+      <c r="BZ10" s="4">
+        <v>0</v>
+      </c>
+      <c r="CA10" s="4">
+        <v>0</v>
+      </c>
+      <c r="CB10" s="4">
+        <v>0</v>
+      </c>
+      <c r="CC10" s="4">
+        <v>0</v>
+      </c>
+      <c r="CD10" s="4">
+        <v>0</v>
+      </c>
+      <c r="CE10" s="4">
+        <v>0</v>
+      </c>
+      <c r="CF10" s="4">
+        <v>0</v>
+      </c>
+      <c r="CG10" s="4">
+        <v>0</v>
+      </c>
+      <c r="CH10" s="4">
+        <v>0</v>
+      </c>
+      <c r="CI10" s="4">
+        <v>0</v>
+      </c>
+      <c r="CJ10" s="4">
+        <v>0</v>
+      </c>
+      <c r="CK10" s="4">
+        <v>0</v>
+      </c>
+      <c r="CL10" s="4">
+        <v>0</v>
+      </c>
+      <c r="CM10" s="4">
+        <v>0</v>
+      </c>
+      <c r="CN10" s="4">
+        <v>0</v>
+      </c>
+      <c r="CO10" s="4">
+        <v>0</v>
+      </c>
+      <c r="CP10" s="4">
+        <v>0</v>
+      </c>
+      <c r="CQ10" s="4">
+        <v>0</v>
+      </c>
+      <c r="CR10" s="4">
+        <v>0</v>
+      </c>
+      <c r="CS10" s="4">
+        <v>0</v>
+      </c>
+      <c r="CT10" s="4">
+        <v>0</v>
+      </c>
+      <c r="CU10" s="4">
+        <v>0</v>
+      </c>
+      <c r="CV10" s="4">
+        <v>0</v>
+      </c>
+      <c r="CW10" s="4">
+        <v>0</v>
+      </c>
+      <c r="CX10" s="4">
+        <v>0</v>
+      </c>
+      <c r="CY10" s="4">
+        <v>0</v>
+      </c>
+      <c r="CZ10" s="4">
+        <v>0</v>
+      </c>
+      <c r="DA10" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="2:105" x14ac:dyDescent="0.25">
       <c r="B11" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="C11" s="4">
+        <v>1</v>
+      </c>
+      <c r="D11" s="4">
+        <v>1</v>
+      </c>
+      <c r="E11" s="4">
+        <v>1</v>
+      </c>
+      <c r="F11" s="4">
+        <v>1</v>
+      </c>
+      <c r="G11" s="4">
+        <v>1</v>
+      </c>
+      <c r="H11" s="4">
+        <v>1</v>
+      </c>
+      <c r="I11" s="4">
+        <v>1</v>
+      </c>
+      <c r="J11" s="4">
+        <v>2</v>
+      </c>
+      <c r="K11" s="4">
+        <v>2</v>
+      </c>
+      <c r="L11" s="4">
+        <v>2</v>
+      </c>
+      <c r="M11" s="4">
+        <v>2</v>
+      </c>
+      <c r="N11" s="4">
+        <v>2</v>
+      </c>
+      <c r="O11" s="4">
+        <v>1</v>
+      </c>
+      <c r="P11" s="4">
+        <v>1</v>
+      </c>
+      <c r="Q11" s="4">
+        <v>1</v>
+      </c>
+      <c r="R11" s="4">
+        <v>1</v>
+      </c>
+      <c r="S11" s="4">
+        <v>1</v>
+      </c>
+      <c r="T11" s="4">
+        <v>1</v>
+      </c>
+      <c r="U11" s="4">
+        <v>2</v>
+      </c>
+      <c r="V11" s="4">
+        <v>2</v>
+      </c>
+      <c r="W11" s="4">
+        <v>2</v>
+      </c>
+      <c r="X11" s="4">
+        <v>2</v>
+      </c>
+      <c r="Y11" s="4">
+        <v>2</v>
+      </c>
+      <c r="Z11" s="4">
+        <v>2</v>
+      </c>
+      <c r="AA11" s="4">
+        <v>2</v>
+      </c>
+      <c r="AB11" s="4">
+        <v>2</v>
+      </c>
+      <c r="AC11" s="4">
+        <v>2</v>
+      </c>
+      <c r="AD11" s="4">
+        <v>1</v>
+      </c>
+      <c r="AE11" s="4">
+        <v>1</v>
+      </c>
+      <c r="AF11" s="4">
+        <v>2</v>
+      </c>
+      <c r="AG11" s="4">
+        <v>2</v>
+      </c>
+      <c r="AH11" s="4">
+        <v>2</v>
+      </c>
+      <c r="AI11" s="4">
+        <v>2</v>
+      </c>
+      <c r="AJ11" s="4">
+        <v>2</v>
+      </c>
+      <c r="AK11" s="4">
+        <v>2</v>
+      </c>
+      <c r="AL11" s="4">
+        <v>2</v>
+      </c>
+      <c r="AM11" s="4">
+        <v>2</v>
+      </c>
+      <c r="AN11" s="4">
+        <v>2</v>
+      </c>
+      <c r="AO11" s="4">
+        <v>2</v>
+      </c>
+      <c r="AP11" s="4">
+        <v>2</v>
+      </c>
+      <c r="AQ11" s="4">
+        <v>2</v>
+      </c>
+      <c r="AR11" s="4">
+        <v>1</v>
+      </c>
+      <c r="AS11" s="4">
+        <v>1</v>
+      </c>
+      <c r="AT11" s="4">
+        <v>1</v>
+      </c>
+      <c r="AU11" s="4">
+        <v>1</v>
+      </c>
+      <c r="AV11" s="4">
+        <v>1</v>
+      </c>
+      <c r="AW11" s="4">
+        <v>1</v>
+      </c>
+      <c r="AX11" s="4">
+        <v>2</v>
+      </c>
+      <c r="AY11" s="4">
+        <v>1</v>
+      </c>
+      <c r="AZ11" s="4">
+        <v>2</v>
+      </c>
+      <c r="BA11" s="4">
+        <v>2</v>
+      </c>
+      <c r="BB11" s="4">
+        <v>2</v>
+      </c>
+      <c r="BC11" s="4">
+        <v>1</v>
+      </c>
+      <c r="BD11" s="4">
+        <v>1</v>
+      </c>
+      <c r="BE11" s="4">
+        <v>1</v>
+      </c>
+      <c r="BF11" s="4">
+        <v>1</v>
+      </c>
+      <c r="BG11" s="4">
+        <v>2</v>
+      </c>
+      <c r="BH11" s="4">
+        <v>2</v>
+      </c>
+      <c r="BI11" s="4">
+        <v>2</v>
+      </c>
+      <c r="BJ11" s="4">
+        <v>2</v>
+      </c>
+      <c r="BK11" s="4">
+        <v>1</v>
+      </c>
+      <c r="BL11" s="4">
+        <v>1</v>
+      </c>
+      <c r="BM11" s="4">
+        <v>1</v>
+      </c>
+      <c r="BN11" s="4">
+        <v>2</v>
+      </c>
+      <c r="BO11" s="4">
+        <v>1</v>
+      </c>
+      <c r="BP11" s="4">
+        <v>1</v>
+      </c>
+      <c r="BQ11" s="4">
+        <v>1</v>
+      </c>
+      <c r="BR11" s="4">
+        <v>1</v>
+      </c>
+      <c r="BS11" s="4">
+        <v>1</v>
+      </c>
+      <c r="BT11" s="4">
+        <v>2</v>
+      </c>
+      <c r="BU11" s="4">
+        <v>2</v>
+      </c>
+      <c r="BV11" s="4">
+        <v>2</v>
+      </c>
+      <c r="BW11" s="4">
+        <v>2</v>
+      </c>
+      <c r="BX11" s="4">
+        <v>2</v>
+      </c>
+      <c r="BY11" s="4">
+        <v>2</v>
+      </c>
+      <c r="BZ11" s="4">
+        <v>2</v>
+      </c>
+      <c r="CA11" s="4">
+        <v>2</v>
+      </c>
+      <c r="CB11" s="4">
+        <v>2</v>
+      </c>
+      <c r="CC11" s="4">
+        <v>2</v>
+      </c>
+      <c r="CD11" s="4">
+        <v>2</v>
+      </c>
+      <c r="CE11" s="4">
+        <v>2</v>
+      </c>
+      <c r="CF11" s="4">
+        <v>2</v>
+      </c>
+      <c r="CG11" s="4">
+        <v>1</v>
+      </c>
+      <c r="CH11" s="4">
+        <v>1</v>
+      </c>
+      <c r="CI11" s="4">
+        <v>1</v>
+      </c>
+      <c r="CJ11" s="4">
+        <v>1</v>
+      </c>
+      <c r="CK11" s="4">
+        <v>1</v>
+      </c>
+      <c r="CL11" s="4">
+        <v>1</v>
+      </c>
+      <c r="CM11" s="4">
+        <v>1</v>
+      </c>
+      <c r="CN11" s="4">
+        <v>1</v>
+      </c>
+      <c r="CO11" s="4">
+        <v>2</v>
+      </c>
+      <c r="CP11" s="4">
+        <v>2</v>
+      </c>
+      <c r="CQ11" s="4">
+        <v>2</v>
+      </c>
+      <c r="CR11" s="4">
+        <v>1</v>
+      </c>
+      <c r="CS11" s="4">
+        <v>1</v>
+      </c>
+      <c r="CT11" s="4">
+        <v>1</v>
+      </c>
+      <c r="CU11" s="4">
+        <v>2</v>
+      </c>
+      <c r="CV11" s="4">
+        <v>1</v>
+      </c>
+      <c r="CW11" s="4">
+        <v>2</v>
+      </c>
+      <c r="CX11" s="4">
+        <v>1</v>
+      </c>
+      <c r="CY11" s="4">
+        <v>2</v>
+      </c>
+      <c r="CZ11" s="4">
+        <v>1</v>
+      </c>
+      <c r="DA11" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="2:105" x14ac:dyDescent="0.25">
+      <c r="B12" s="3" t="s">
         <v>37</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="E11" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="F11" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="G11" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="H11" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="I11" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="J11" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="K11" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="L11" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="M11" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="N11" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="O11" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="P11" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="Q11" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="R11" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="S11" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="T11" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="U11" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="V11" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="W11" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="X11" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="Y11" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="Z11" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="AA11" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="AB11" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="AC11" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="AD11" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="AE11" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="AF11" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="AG11" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="AH11" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="AI11" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="AJ11" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="AK11" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="AL11" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="AM11" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="AN11" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="AO11" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="AP11" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="AQ11" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="AR11" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="AS11" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="AT11" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="AU11" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="AV11" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="AW11" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="AX11" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="AY11" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="AZ11" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="BA11" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="BB11" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="BC11" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="BD11" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="BE11" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="BF11" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="BG11" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="BH11" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="BI11" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="BJ11" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="BK11" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="BL11" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="BM11" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="BN11" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="BO11" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="BP11" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="BQ11" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="BR11" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="BS11" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="BT11" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="BU11" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="BV11" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="BW11" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="BX11" s="4" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="12" spans="2:76" x14ac:dyDescent="0.25">
-      <c r="B12" s="3" t="s">
-        <v>39</v>
       </c>
       <c r="C12" s="4">
         <v>1</v>
@@ -3069,10 +3782,97 @@
       <c r="BX12" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="2:76" x14ac:dyDescent="0.25">
+      <c r="BY12" s="4">
+        <v>0</v>
+      </c>
+      <c r="BZ12" s="4">
+        <v>0</v>
+      </c>
+      <c r="CA12" s="4">
+        <v>0</v>
+      </c>
+      <c r="CB12" s="4">
+        <v>0</v>
+      </c>
+      <c r="CC12" s="4">
+        <v>0</v>
+      </c>
+      <c r="CD12" s="4">
+        <v>0</v>
+      </c>
+      <c r="CE12" s="4">
+        <v>0</v>
+      </c>
+      <c r="CF12" s="4">
+        <v>0</v>
+      </c>
+      <c r="CG12" s="4">
+        <v>0</v>
+      </c>
+      <c r="CH12" s="4">
+        <v>0</v>
+      </c>
+      <c r="CI12" s="4">
+        <v>0</v>
+      </c>
+      <c r="CJ12" s="4">
+        <v>0</v>
+      </c>
+      <c r="CK12" s="4">
+        <v>0</v>
+      </c>
+      <c r="CL12" s="4">
+        <v>0</v>
+      </c>
+      <c r="CM12" s="4">
+        <v>0</v>
+      </c>
+      <c r="CN12" s="4">
+        <v>0</v>
+      </c>
+      <c r="CO12" s="4">
+        <v>0</v>
+      </c>
+      <c r="CP12" s="4">
+        <v>0</v>
+      </c>
+      <c r="CQ12" s="4">
+        <v>0</v>
+      </c>
+      <c r="CR12" s="4">
+        <v>0</v>
+      </c>
+      <c r="CS12" s="4">
+        <v>0</v>
+      </c>
+      <c r="CT12" s="4">
+        <v>0</v>
+      </c>
+      <c r="CU12" s="4">
+        <v>0</v>
+      </c>
+      <c r="CV12" s="4">
+        <v>0</v>
+      </c>
+      <c r="CW12" s="4">
+        <v>0</v>
+      </c>
+      <c r="CX12" s="4">
+        <v>0</v>
+      </c>
+      <c r="CY12" s="4">
+        <v>0</v>
+      </c>
+      <c r="CZ12" s="4">
+        <v>0</v>
+      </c>
+      <c r="DA12" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="2:105" x14ac:dyDescent="0.25">
       <c r="B13" s="3" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C13" s="4"/>
       <c r="D13" s="4">
@@ -3164,17 +3964,46 @@
       <c r="BV13" s="4"/>
       <c r="BW13" s="4"/>
       <c r="BX13" s="4"/>
-    </row>
-    <row r="14" spans="2:76" x14ac:dyDescent="0.25">
+      <c r="BY13" s="4"/>
+      <c r="BZ13" s="4"/>
+      <c r="CA13" s="4"/>
+      <c r="CB13" s="4"/>
+      <c r="CC13" s="4"/>
+      <c r="CD13" s="4"/>
+      <c r="CE13" s="4"/>
+      <c r="CF13" s="4"/>
+      <c r="CG13" s="4"/>
+      <c r="CH13" s="4"/>
+      <c r="CI13" s="4"/>
+      <c r="CJ13" s="4"/>
+      <c r="CK13" s="4"/>
+      <c r="CL13" s="4"/>
+      <c r="CM13" s="4"/>
+      <c r="CN13" s="4"/>
+      <c r="CO13" s="4"/>
+      <c r="CP13" s="4"/>
+      <c r="CQ13" s="4"/>
+      <c r="CR13" s="4"/>
+      <c r="CS13" s="4"/>
+      <c r="CT13" s="4"/>
+      <c r="CU13" s="4"/>
+      <c r="CV13" s="4"/>
+      <c r="CW13" s="4"/>
+      <c r="CX13" s="4"/>
+      <c r="CY13" s="4"/>
+      <c r="CZ13" s="4"/>
+      <c r="DA13" s="4"/>
+    </row>
+    <row r="14" spans="2:105" x14ac:dyDescent="0.25">
       <c r="B14" s="6" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="AB14" s="7"/>
       <c r="AC14" s="7"/>
     </row>
-    <row r="15" spans="2:76" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:105" x14ac:dyDescent="0.25">
       <c r="B15" s="6" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="O15">
         <v>1</v>
@@ -3215,32 +4044,64 @@
     </row>
     <row r="19" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="24" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="25" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="26" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="27" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="28" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
-        <v>152</v>
+        <v>150</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15496ECB-863E-462B-A169-809C8D88AE1B}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>202</v>
       </c>
     </row>
   </sheetData>
@@ -3248,11 +4109,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
+    <sheetView topLeftCell="A41" workbookViewId="0">
       <selection activeCell="F61" sqref="F61"/>
     </sheetView>
   </sheetViews>
@@ -3283,7 +4144,7 @@
         <v>3</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -3300,10 +4161,10 @@
         <v>7</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -3320,10 +4181,10 @@
         <v>7</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -3340,10 +4201,10 @@
         <v>7</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -3360,10 +4221,10 @@
         <v>7</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -3380,10 +4241,10 @@
         <v>7</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -3400,10 +4261,10 @@
         <v>7</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -3420,10 +4281,10 @@
         <v>7</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -3440,10 +4301,10 @@
         <v>8</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -3460,10 +4321,10 @@
         <v>8</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -3480,10 +4341,10 @@
         <v>8</v>
       </c>
       <c r="E11" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="F11" s="1" t="s">
         <v>41</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -3500,10 +4361,10 @@
         <v>8</v>
       </c>
       <c r="E12" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F12" s="1" t="s">
         <v>42</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -3520,10 +4381,10 @@
         <v>8</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -3734,16 +4595,16 @@
         <v>4</v>
       </c>
       <c r="C26" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D26" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
@@ -3751,19 +4612,19 @@
         <v>26</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D27" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
@@ -3771,19 +4632,19 @@
         <v>27</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D28" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E28" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="F28" s="1" t="s">
         <v>73</v>
-      </c>
-      <c r="F28" s="1" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
@@ -3791,19 +4652,19 @@
         <v>28</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="D29" s="1" t="s">
         <v>7</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
@@ -3811,19 +4672,19 @@
         <v>29</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="D30" s="1" t="s">
         <v>7</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
@@ -3831,19 +4692,19 @@
         <v>30</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D31" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
@@ -3851,19 +4712,19 @@
         <v>31</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D32" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
@@ -3871,19 +4732,19 @@
         <v>32</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D33" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
@@ -3891,19 +4752,19 @@
         <v>33</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D34" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
@@ -3911,19 +4772,19 @@
         <v>34</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D35" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
@@ -3931,19 +4792,19 @@
         <v>35</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="D36" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
@@ -3951,19 +4812,19 @@
         <v>36</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D37" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
@@ -3971,19 +4832,19 @@
         <v>37</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D38" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
@@ -3991,19 +4852,19 @@
         <v>38</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D39" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
@@ -4011,19 +4872,19 @@
         <v>39</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D40" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
@@ -4031,19 +4892,19 @@
         <v>40</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D41" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
@@ -4051,19 +4912,19 @@
         <v>41</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D42" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
@@ -4071,19 +4932,19 @@
         <v>42</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C43" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E43" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="D43" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E43" s="1" t="s">
-        <v>117</v>
-      </c>
       <c r="F43" s="1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
@@ -4091,19 +4952,19 @@
         <v>43</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D44" s="1" t="s">
         <v>7</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
@@ -4111,19 +4972,19 @@
         <v>44</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="D45" s="1" t="s">
         <v>7</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
@@ -4131,19 +4992,19 @@
         <v>45</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="D46" s="1" t="s">
         <v>7</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
@@ -4151,19 +5012,19 @@
         <v>46</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="D47" s="1" t="s">
         <v>7</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
@@ -4171,19 +5032,19 @@
         <v>47</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="D48" s="1" t="s">
         <v>7</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
@@ -4191,19 +5052,19 @@
         <v>48</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="D49" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E49" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="F49" s="1" t="s">
         <v>129</v>
-      </c>
-      <c r="F49" s="1" t="s">
-        <v>131</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
@@ -4211,19 +5072,19 @@
         <v>49</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C50" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E50" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="F50" s="1" t="s">
         <v>134</v>
-      </c>
-      <c r="D50" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E50" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="F50" s="1" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
@@ -4231,19 +5092,19 @@
         <v>50</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="D51" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E51" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="F51" t="s">
         <v>138</v>
-      </c>
-      <c r="F51" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
@@ -4251,19 +5112,19 @@
         <v>51</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="D52" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
@@ -4271,19 +5132,19 @@
         <v>52</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="D53" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="F53" s="1" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
@@ -4291,19 +5152,19 @@
         <v>53</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C54" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="D54" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E54" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="D54" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E54" s="1" t="s">
-        <v>150</v>
-      </c>
       <c r="F54" s="1" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
@@ -4311,19 +5172,19 @@
         <v>54</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="D55" s="1" t="s">
         <v>7</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="F55" s="1" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
@@ -4331,19 +5192,19 @@
         <v>55</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="D56" s="1" t="s">
         <v>7</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="F56" s="1" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
@@ -4351,19 +5212,19 @@
         <v>56</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="D57" s="1" t="s">
         <v>7</v>
       </c>
       <c r="E57" s="1" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="F57" s="1" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
@@ -4371,19 +5232,19 @@
         <v>57</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="D58" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="F58" s="1" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
@@ -4391,19 +5252,19 @@
         <v>58</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="D59" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="F59" s="1" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
@@ -4411,19 +5272,19 @@
         <v>59</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="D60" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="F60" s="1" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
@@ -4431,19 +5292,19 @@
         <v>60</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C61" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D61" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="F61" s="1" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
@@ -4451,19 +5312,19 @@
         <v>61</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C62" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D62" s="1" t="s">
         <v>7</v>
       </c>
       <c r="E62" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="F62" s="1" t="s">
         <v>172</v>
-      </c>
-      <c r="F62" s="1" t="s">
-        <v>174</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
@@ -4471,19 +5332,19 @@
         <v>62</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C63" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="D63" s="1" t="s">
         <v>7</v>
       </c>
       <c r="E63" s="1" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="F63" s="1" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
@@ -4491,19 +5352,19 @@
         <v>63</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C64" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="D64" s="1" t="s">
         <v>7</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="F64" s="1" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
@@ -4511,19 +5372,19 @@
         <v>64</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C65" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="D65" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="F65" s="1" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
@@ -4531,16 +5392,16 @@
         <v>65</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="C66" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="D66" s="1" t="s">
         <v>7</v>
       </c>
       <c r="E66" s="1" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
@@ -4548,10 +5409,10 @@
         <v>66</v>
       </c>
       <c r="B67" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="C67" t="s">
         <v>185</v>
-      </c>
-      <c r="C67" t="s">
-        <v>187</v>
       </c>
       <c r="D67" s="1" t="s">
         <v>7</v>
@@ -4562,10 +5423,10 @@
         <v>67</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="C68" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="D68" s="1" t="s">
         <v>7</v>
@@ -4576,10 +5437,10 @@
         <v>68</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="C69" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="D69" s="1" t="s">
         <v>7</v>
@@ -4590,10 +5451,10 @@
         <v>69</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="C70" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="D70" s="1" t="s">
         <v>7</v>
@@ -4604,10 +5465,10 @@
         <v>70</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="C71" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="D71" s="1" t="s">
         <v>8</v>
@@ -4618,10 +5479,10 @@
         <v>71</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="C72" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="D72" s="1" t="s">
         <v>8</v>
@@ -4632,10 +5493,10 @@
         <v>72</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="C73" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D73" s="1" t="s">
         <v>8</v>
@@ -4646,10 +5507,10 @@
         <v>73</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="C74" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="D74" s="1" t="s">
         <v>8</v>
@@ -4660,10 +5521,10 @@
         <v>74</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="C75" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="D75" s="1" t="s">
         <v>8</v>
@@ -4675,7 +5536,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A6C2E3B-6ECE-4AF1-B74E-2ADC4D0D5D0C}">
   <dimension ref="A1:B4"/>
   <sheetViews>
@@ -4690,7 +5551,7 @@
         <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -4698,7 +5559,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -4706,7 +5567,7 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -4714,7 +5575,7 @@
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
   </sheetData>
@@ -4722,12 +5583,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25CB833E-39AA-47F0-B506-E40379BB6129}">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4737,7 +5598,7 @@
         <v>1</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -4745,7 +5606,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -4753,7 +5614,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -4761,10 +5622,10 @@
         <v>5</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C5" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -4772,15 +5633,26 @@
         <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>51</v>
-      </c>
+        <v>49</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>7</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B9" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6499CB2B-6832-4092-A9EA-DD66A17F48BA}">
   <dimension ref="A1:B12"/>
   <sheetViews>
@@ -4795,7 +5667,7 @@
         <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -4803,7 +5675,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -4811,7 +5683,7 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -4819,7 +5691,7 @@
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -4827,7 +5699,7 @@
         <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -4835,7 +5707,7 @@
         <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -4843,7 +5715,7 @@
         <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -4851,7 +5723,7 @@
         <v>8</v>
       </c>
       <c r="B8" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -4859,7 +5731,7 @@
         <v>9</v>
       </c>
       <c r="B9" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -4867,7 +5739,7 @@
         <v>10</v>
       </c>
       <c r="B10" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -4875,7 +5747,7 @@
         <v>11</v>
       </c>
       <c r="B11" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -4883,7 +5755,7 @@
         <v>12</v>
       </c>
       <c r="B12" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: Added lab2 which separates single-cell datasets to the design matrix
</commit_message>
<xml_diff>
--- a/DesignMatrix.xlsx
+++ b/DesignMatrix.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFA26531-BE5D-4C8A-8827-C768A72DFB39}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B35DBE4-F70C-41BD-8752-653BF79919A8}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DesignMatrix" sheetId="2" r:id="rId1"/>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="387" uniqueCount="205">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="389" uniqueCount="208">
   <si>
     <t>Sample index</t>
   </si>
@@ -663,6 +663,15 @@
   </si>
   <si>
     <t>10x pooled single-cell</t>
+  </si>
+  <si>
+    <t>Cell type B=1</t>
+  </si>
+  <si>
+    <t>Lab2 (ss separate labs)</t>
+  </si>
+  <si>
+    <t>the last 3 are different labs, but we only have one sample per dataset</t>
   </si>
 </sst>
 </file>
@@ -1049,10 +1058,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F369D9C3-2B00-4B3E-B4DE-89D514952C05}">
-  <dimension ref="B2:DA28"/>
+  <dimension ref="B2:DA29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AP1" workbookViewId="0">
-      <selection activeCell="BY4" sqref="BY4:DA4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" activeCellId="1" sqref="B4 B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3258,7 +3267,7 @@
     </row>
     <row r="11" spans="2:105" x14ac:dyDescent="0.25">
       <c r="B11" s="3" t="s">
-        <v>5</v>
+        <v>205</v>
       </c>
       <c r="C11" s="4">
         <v>1</v>
@@ -3986,79 +3995,396 @@
     </row>
     <row r="14" spans="2:105" x14ac:dyDescent="0.25">
       <c r="B14" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="AB14" s="7"/>
-      <c r="AC14" s="7"/>
+        <v>206</v>
+      </c>
+      <c r="C14" s="4">
+        <v>2</v>
+      </c>
+      <c r="D14" s="4">
+        <v>3</v>
+      </c>
+      <c r="E14" s="4">
+        <v>3</v>
+      </c>
+      <c r="F14" s="4">
+        <v>3</v>
+      </c>
+      <c r="G14" s="4">
+        <v>3</v>
+      </c>
+      <c r="H14" s="4">
+        <v>3</v>
+      </c>
+      <c r="I14" s="4">
+        <v>3</v>
+      </c>
+      <c r="J14" s="4">
+        <v>2</v>
+      </c>
+      <c r="K14" s="4">
+        <v>2</v>
+      </c>
+      <c r="L14" s="4">
+        <v>2</v>
+      </c>
+      <c r="M14" s="4">
+        <v>2</v>
+      </c>
+      <c r="N14" s="4">
+        <v>2</v>
+      </c>
+      <c r="O14" s="5">
+        <v>4</v>
+      </c>
+      <c r="P14" s="5">
+        <v>4</v>
+      </c>
+      <c r="Q14" s="5">
+        <v>4</v>
+      </c>
+      <c r="R14" s="5">
+        <v>4</v>
+      </c>
+      <c r="S14" s="5">
+        <v>4</v>
+      </c>
+      <c r="T14" s="5">
+        <v>4</v>
+      </c>
+      <c r="U14" s="5">
+        <v>4</v>
+      </c>
+      <c r="V14" s="5">
+        <v>4</v>
+      </c>
+      <c r="W14" s="5">
+        <v>4</v>
+      </c>
+      <c r="X14" s="5">
+        <v>4</v>
+      </c>
+      <c r="Y14" s="5">
+        <v>4</v>
+      </c>
+      <c r="Z14" s="5">
+        <v>4</v>
+      </c>
+      <c r="AA14" s="5">
+        <v>2</v>
+      </c>
+      <c r="AB14" s="5">
+        <v>5</v>
+      </c>
+      <c r="AC14" s="5">
+        <v>5</v>
+      </c>
+      <c r="AD14" s="5">
+        <v>5</v>
+      </c>
+      <c r="AE14" s="5">
+        <v>5</v>
+      </c>
+      <c r="AF14" s="5">
+        <v>5</v>
+      </c>
+      <c r="AG14" s="5">
+        <v>5</v>
+      </c>
+      <c r="AH14" s="5">
+        <v>5</v>
+      </c>
+      <c r="AI14" s="5">
+        <v>5</v>
+      </c>
+      <c r="AJ14" s="5">
+        <v>5</v>
+      </c>
+      <c r="AK14" s="5">
+        <v>5</v>
+      </c>
+      <c r="AL14" s="5">
+        <v>5</v>
+      </c>
+      <c r="AM14" s="5">
+        <v>5</v>
+      </c>
+      <c r="AN14" s="5">
+        <v>5</v>
+      </c>
+      <c r="AO14" s="5">
+        <v>5</v>
+      </c>
+      <c r="AP14" s="5">
+        <v>5</v>
+      </c>
+      <c r="AQ14" s="5">
+        <v>5</v>
+      </c>
+      <c r="AR14" s="4">
+        <v>5</v>
+      </c>
+      <c r="AS14" s="4">
+        <v>5</v>
+      </c>
+      <c r="AT14" s="4">
+        <v>5</v>
+      </c>
+      <c r="AU14" s="4">
+        <v>5</v>
+      </c>
+      <c r="AV14" s="4">
+        <v>5</v>
+      </c>
+      <c r="AW14" s="4">
+        <v>5</v>
+      </c>
+      <c r="AX14" s="4">
+        <v>5</v>
+      </c>
+      <c r="AY14" s="4">
+        <v>5</v>
+      </c>
+      <c r="AZ14" s="4">
+        <v>5</v>
+      </c>
+      <c r="BA14" s="4">
+        <v>5</v>
+      </c>
+      <c r="BB14" s="4">
+        <v>5</v>
+      </c>
+      <c r="BC14" s="4">
+        <v>5</v>
+      </c>
+      <c r="BD14" s="4">
+        <v>5</v>
+      </c>
+      <c r="BE14" s="4">
+        <v>5</v>
+      </c>
+      <c r="BF14" s="4">
+        <v>5</v>
+      </c>
+      <c r="BG14" s="4">
+        <v>5</v>
+      </c>
+      <c r="BH14" s="4">
+        <v>5</v>
+      </c>
+      <c r="BI14" s="4">
+        <v>5</v>
+      </c>
+      <c r="BJ14" s="4">
+        <v>5</v>
+      </c>
+      <c r="BK14" s="4">
+        <v>5</v>
+      </c>
+      <c r="BL14" s="4">
+        <v>5</v>
+      </c>
+      <c r="BM14" s="4">
+        <v>5</v>
+      </c>
+      <c r="BN14" s="4">
+        <v>5</v>
+      </c>
+      <c r="BO14" s="4">
+        <v>1</v>
+      </c>
+      <c r="BP14" s="4">
+        <v>1</v>
+      </c>
+      <c r="BQ14" s="4">
+        <v>1</v>
+      </c>
+      <c r="BR14" s="4">
+        <v>1</v>
+      </c>
+      <c r="BS14" s="4">
+        <v>1</v>
+      </c>
+      <c r="BT14" s="4">
+        <v>1</v>
+      </c>
+      <c r="BU14" s="4">
+        <v>1</v>
+      </c>
+      <c r="BV14" s="4">
+        <v>1</v>
+      </c>
+      <c r="BW14" s="4">
+        <v>1</v>
+      </c>
+      <c r="BX14" s="4">
+        <v>1</v>
+      </c>
+      <c r="BY14" s="4">
+        <v>6</v>
+      </c>
+      <c r="BZ14" s="4">
+        <v>6</v>
+      </c>
+      <c r="CA14" s="4">
+        <v>6</v>
+      </c>
+      <c r="CB14" s="4">
+        <v>6</v>
+      </c>
+      <c r="CC14" s="4">
+        <v>6</v>
+      </c>
+      <c r="CD14" s="4">
+        <v>6</v>
+      </c>
+      <c r="CE14" s="4">
+        <v>6</v>
+      </c>
+      <c r="CF14" s="4">
+        <v>6</v>
+      </c>
+      <c r="CG14" s="4">
+        <v>6</v>
+      </c>
+      <c r="CH14" s="4">
+        <v>6</v>
+      </c>
+      <c r="CI14" s="4">
+        <v>6</v>
+      </c>
+      <c r="CJ14" s="4">
+        <v>6</v>
+      </c>
+      <c r="CK14" s="4">
+        <v>6</v>
+      </c>
+      <c r="CL14" s="4">
+        <v>6</v>
+      </c>
+      <c r="CM14" s="4">
+        <v>6</v>
+      </c>
+      <c r="CN14" s="4">
+        <v>6</v>
+      </c>
+      <c r="CO14" s="4">
+        <v>7</v>
+      </c>
+      <c r="CP14" s="4">
+        <v>7</v>
+      </c>
+      <c r="CQ14" s="4">
+        <v>7</v>
+      </c>
+      <c r="CR14" s="4">
+        <v>7</v>
+      </c>
+      <c r="CS14" s="4">
+        <v>7</v>
+      </c>
+      <c r="CT14" s="4">
+        <v>7</v>
+      </c>
+      <c r="CU14" s="4">
+        <v>7</v>
+      </c>
+      <c r="CV14" s="4">
+        <v>7</v>
+      </c>
+      <c r="CW14" s="4">
+        <v>8</v>
+      </c>
+      <c r="CX14" s="4">
+        <v>8</v>
+      </c>
+      <c r="CY14" s="4">
+        <v>9</v>
+      </c>
+      <c r="CZ14" s="4">
+        <v>9</v>
+      </c>
+      <c r="DA14" s="4">
+        <v>9</v>
+      </c>
     </row>
     <row r="15" spans="2:105" x14ac:dyDescent="0.25">
       <c r="B15" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="AB15" s="7"/>
+      <c r="AC15" s="7"/>
+    </row>
+    <row r="16" spans="2:105" x14ac:dyDescent="0.25">
+      <c r="B16" s="6" t="s">
         <v>195</v>
       </c>
-      <c r="O15">
-        <v>1</v>
-      </c>
-      <c r="P15">
-        <v>1</v>
-      </c>
-      <c r="Q15">
-        <v>1</v>
-      </c>
-      <c r="R15">
-        <v>1</v>
-      </c>
-      <c r="S15">
-        <v>1</v>
-      </c>
-      <c r="T15">
-        <v>1</v>
-      </c>
-      <c r="U15">
-        <v>1</v>
-      </c>
-      <c r="V15">
-        <v>1</v>
-      </c>
-      <c r="W15">
-        <v>1</v>
-      </c>
-      <c r="X15">
-        <v>1</v>
-      </c>
-      <c r="Y15">
-        <v>1</v>
-      </c>
-      <c r="Z15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B19" t="s">
+      <c r="O16">
+        <v>1</v>
+      </c>
+      <c r="P16">
+        <v>1</v>
+      </c>
+      <c r="Q16">
+        <v>1</v>
+      </c>
+      <c r="R16">
+        <v>1</v>
+      </c>
+      <c r="S16">
+        <v>1</v>
+      </c>
+      <c r="T16">
+        <v>1</v>
+      </c>
+      <c r="U16">
+        <v>1</v>
+      </c>
+      <c r="V16">
+        <v>1</v>
+      </c>
+      <c r="W16">
+        <v>1</v>
+      </c>
+      <c r="X16">
+        <v>1</v>
+      </c>
+      <c r="Y16">
+        <v>1</v>
+      </c>
+      <c r="Z16">
+        <v>1</v>
+      </c>
+      <c r="CY16" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
         <v>64</v>
-      </c>
-    </row>
-    <row r="24" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B24" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="25" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="26" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
-        <v>111</v>
+        <v>69</v>
       </c>
     </row>
     <row r="27" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
-        <v>131</v>
+        <v>111</v>
       </c>
     </row>
     <row r="28" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="29" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B29" t="s">
         <v>150</v>
       </c>
     </row>

</xml_diff>

<commit_message>
feat: Made some progress. Have a draft version of figure 1 and 2. Also added the melanoma dataset and restructured the design matrix a bit.
</commit_message>
<xml_diff>
--- a/DesignMatrix.xlsx
+++ b/DesignMatrix.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B35DBE4-F70C-41BD-8752-653BF79919A8}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58618146-0CAE-44F7-A3BE-C20F3A5A0687}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,6 +23,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -48,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="389" uniqueCount="208">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="391" uniqueCount="210">
   <si>
     <t>Sample index</t>
   </si>
@@ -236,9 +237,6 @@
     <t>Technical Replicates</t>
   </si>
   <si>
-    <t>Gingeras</t>
-  </si>
-  <si>
     <t>ENCBS424MFE</t>
   </si>
   <si>
@@ -593,12 +591,6 @@
     <t>Central memory CD8+ T cell</t>
   </si>
   <si>
-    <t>Sauvageau (GSE 51984)</t>
-  </si>
-  <si>
-    <t>John Stamatoyannopoulos, Zhiping Weng, UMass</t>
-  </si>
-  <si>
     <t>GSE 51984</t>
   </si>
   <si>
@@ -662,16 +654,31 @@
     <t>Single-cell</t>
   </si>
   <si>
-    <t>10x pooled single-cell</t>
-  </si>
-  <si>
     <t>Cell type B=1</t>
   </si>
   <si>
-    <t>Lab2 (ss separate labs)</t>
-  </si>
-  <si>
-    <t>the last 3 are different labs, but we only have one sample per dataset</t>
+    <t>Pabst, Sauvageau (GSE 51984)</t>
+  </si>
+  <si>
+    <t>ENCODE: John Stamatoyannopoulos, Zhiping Weng, UMass</t>
+  </si>
+  <si>
+    <t>ENCODE: Gingeras</t>
+  </si>
+  <si>
+    <t>Pooled single-cell, PBMC, 10x data</t>
+  </si>
+  <si>
+    <t>Pooled single-cell, Tirosh et al, Melanoma, SmartSeq2</t>
+  </si>
+  <si>
+    <t>Pooled single-cell, 68k PBMC, 10x data</t>
+  </si>
+  <si>
+    <t>Pooled single-cell, Lung cancer, 10x data, Lambrechts et al</t>
+  </si>
+  <si>
+    <t>Pooled single-cell, Cord blood, Human Cell Atlas</t>
   </si>
 </sst>
 </file>
@@ -1058,20 +1065,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F369D9C3-2B00-4B3E-B4DE-89D514952C05}">
-  <dimension ref="B2:DA29"/>
+  <dimension ref="B2:DC28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" activeCellId="1" sqref="B4 B5"/>
+      <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3.85546875" customWidth="1"/>
     <col min="2" max="2" width="18.85546875" customWidth="1"/>
-    <col min="3" max="105" width="3.85546875" customWidth="1"/>
+    <col min="3" max="107" width="3.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:105" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:107" x14ac:dyDescent="0.25">
       <c r="C2" t="s">
         <v>4</v>
       </c>
@@ -1082,16 +1089,16 @@
         <v>4</v>
       </c>
       <c r="AB2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="BO2" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="BY2" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="3" spans="2:105" x14ac:dyDescent="0.25">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="3" spans="2:107" x14ac:dyDescent="0.25">
       <c r="B3" s="3" t="s">
         <v>29</v>
       </c>
@@ -1404,8 +1411,14 @@
       <c r="DA3" s="3">
         <v>103</v>
       </c>
-    </row>
-    <row r="4" spans="2:105" x14ac:dyDescent="0.25">
+      <c r="DB3" s="3">
+        <v>104</v>
+      </c>
+      <c r="DC3" s="3">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="4" spans="2:107" x14ac:dyDescent="0.25">
       <c r="B4" s="3" t="s">
         <v>28</v>
       </c>
@@ -1680,46 +1693,52 @@
         <v>6</v>
       </c>
       <c r="CO4" s="4">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="CP4" s="4">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="CQ4" s="4">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="CR4" s="4">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="CS4" s="4">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="CT4" s="4">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="CU4" s="4">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="CV4" s="4">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="CW4" s="4">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="CX4" s="4">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="CY4" s="4">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="CZ4" s="4">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="DA4" s="4">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="2:105" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+      <c r="DB4" s="4">
+        <v>10</v>
+      </c>
+      <c r="DC4" s="4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="2:107" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
         <v>30</v>
       </c>
@@ -2032,8 +2051,14 @@
       <c r="DA5" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="2:105" x14ac:dyDescent="0.25">
+      <c r="DB5" s="4">
+        <v>1</v>
+      </c>
+      <c r="DC5" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="2:107" x14ac:dyDescent="0.25">
       <c r="B6" s="3" t="s">
         <v>31</v>
       </c>
@@ -2346,8 +2371,14 @@
       <c r="DA6" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="2:105" x14ac:dyDescent="0.25">
+      <c r="DB6" s="4">
+        <v>1</v>
+      </c>
+      <c r="DC6" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="2:107" x14ac:dyDescent="0.25">
       <c r="B7" s="3" t="s">
         <v>35</v>
       </c>
@@ -2478,8 +2509,10 @@
       <c r="CY7" s="4"/>
       <c r="CZ7" s="4"/>
       <c r="DA7" s="4"/>
-    </row>
-    <row r="8" spans="2:105" x14ac:dyDescent="0.25">
+      <c r="DB7" s="4"/>
+      <c r="DC7" s="4"/>
+    </row>
+    <row r="8" spans="2:107" x14ac:dyDescent="0.25">
       <c r="B8" s="3" t="s">
         <v>43</v>
       </c>
@@ -2636,8 +2669,10 @@
       <c r="CY8" s="4"/>
       <c r="CZ8" s="4"/>
       <c r="DA8" s="4"/>
-    </row>
-    <row r="9" spans="2:105" x14ac:dyDescent="0.25">
+      <c r="DB8" s="4"/>
+      <c r="DC8" s="4"/>
+    </row>
+    <row r="9" spans="2:107" x14ac:dyDescent="0.25">
       <c r="B9" s="3" t="s">
         <v>36</v>
       </c>
@@ -2950,8 +2985,14 @@
       <c r="DA9" s="4">
         <v>2</v>
       </c>
-    </row>
-    <row r="10" spans="2:105" x14ac:dyDescent="0.25">
+      <c r="DB9" s="4">
+        <v>1</v>
+      </c>
+      <c r="DC9" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="2:107" x14ac:dyDescent="0.25">
       <c r="B10" s="3" t="s">
         <v>32</v>
       </c>
@@ -3264,10 +3305,16 @@
       <c r="DA10" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="2:105" x14ac:dyDescent="0.25">
+      <c r="DB10" s="4">
+        <v>0</v>
+      </c>
+      <c r="DC10" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="2:107" x14ac:dyDescent="0.25">
       <c r="B11" s="3" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="C11" s="4">
         <v>1</v>
@@ -3578,8 +3625,14 @@
       <c r="DA11" s="4">
         <v>2</v>
       </c>
-    </row>
-    <row r="12" spans="2:105" x14ac:dyDescent="0.25">
+      <c r="DB11" s="4">
+        <v>2</v>
+      </c>
+      <c r="DC11" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="2:107" x14ac:dyDescent="0.25">
       <c r="B12" s="3" t="s">
         <v>37</v>
       </c>
@@ -3868,8 +3921,14 @@
       <c r="DA12" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="2:105" x14ac:dyDescent="0.25">
+      <c r="DB12" s="4">
+        <v>0</v>
+      </c>
+      <c r="DC12" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="2:107" x14ac:dyDescent="0.25">
       <c r="B13" s="3" t="s">
         <v>61</v>
       </c>
@@ -3992,375 +4051,65 @@
       <c r="CY13" s="4"/>
       <c r="CZ13" s="4"/>
       <c r="DA13" s="4"/>
-    </row>
-    <row r="14" spans="2:105" x14ac:dyDescent="0.25">
+      <c r="DB13" s="4"/>
+      <c r="DC13" s="4"/>
+    </row>
+    <row r="14" spans="2:107" x14ac:dyDescent="0.25">
       <c r="B14" s="6" t="s">
-        <v>206</v>
-      </c>
-      <c r="C14" s="4">
-        <v>2</v>
-      </c>
-      <c r="D14" s="4">
-        <v>3</v>
-      </c>
-      <c r="E14" s="4">
-        <v>3</v>
-      </c>
-      <c r="F14" s="4">
-        <v>3</v>
-      </c>
-      <c r="G14" s="4">
-        <v>3</v>
-      </c>
-      <c r="H14" s="4">
-        <v>3</v>
-      </c>
-      <c r="I14" s="4">
-        <v>3</v>
-      </c>
-      <c r="J14" s="4">
-        <v>2</v>
-      </c>
-      <c r="K14" s="4">
-        <v>2</v>
-      </c>
-      <c r="L14" s="4">
-        <v>2</v>
-      </c>
-      <c r="M14" s="4">
-        <v>2</v>
-      </c>
-      <c r="N14" s="4">
-        <v>2</v>
-      </c>
-      <c r="O14" s="5">
-        <v>4</v>
-      </c>
-      <c r="P14" s="5">
-        <v>4</v>
-      </c>
-      <c r="Q14" s="5">
-        <v>4</v>
-      </c>
-      <c r="R14" s="5">
-        <v>4</v>
-      </c>
-      <c r="S14" s="5">
-        <v>4</v>
-      </c>
-      <c r="T14" s="5">
-        <v>4</v>
-      </c>
-      <c r="U14" s="5">
-        <v>4</v>
-      </c>
-      <c r="V14" s="5">
-        <v>4</v>
-      </c>
-      <c r="W14" s="5">
-        <v>4</v>
-      </c>
-      <c r="X14" s="5">
-        <v>4</v>
-      </c>
-      <c r="Y14" s="5">
-        <v>4</v>
-      </c>
-      <c r="Z14" s="5">
-        <v>4</v>
-      </c>
-      <c r="AA14" s="5">
-        <v>2</v>
-      </c>
-      <c r="AB14" s="5">
-        <v>5</v>
-      </c>
-      <c r="AC14" s="5">
-        <v>5</v>
-      </c>
-      <c r="AD14" s="5">
-        <v>5</v>
-      </c>
-      <c r="AE14" s="5">
-        <v>5</v>
-      </c>
-      <c r="AF14" s="5">
-        <v>5</v>
-      </c>
-      <c r="AG14" s="5">
-        <v>5</v>
-      </c>
-      <c r="AH14" s="5">
-        <v>5</v>
-      </c>
-      <c r="AI14" s="5">
-        <v>5</v>
-      </c>
-      <c r="AJ14" s="5">
-        <v>5</v>
-      </c>
-      <c r="AK14" s="5">
-        <v>5</v>
-      </c>
-      <c r="AL14" s="5">
-        <v>5</v>
-      </c>
-      <c r="AM14" s="5">
-        <v>5</v>
-      </c>
-      <c r="AN14" s="5">
-        <v>5</v>
-      </c>
-      <c r="AO14" s="5">
-        <v>5</v>
-      </c>
-      <c r="AP14" s="5">
-        <v>5</v>
-      </c>
-      <c r="AQ14" s="5">
-        <v>5</v>
-      </c>
-      <c r="AR14" s="4">
-        <v>5</v>
-      </c>
-      <c r="AS14" s="4">
-        <v>5</v>
-      </c>
-      <c r="AT14" s="4">
-        <v>5</v>
-      </c>
-      <c r="AU14" s="4">
-        <v>5</v>
-      </c>
-      <c r="AV14" s="4">
-        <v>5</v>
-      </c>
-      <c r="AW14" s="4">
-        <v>5</v>
-      </c>
-      <c r="AX14" s="4">
-        <v>5</v>
-      </c>
-      <c r="AY14" s="4">
-        <v>5</v>
-      </c>
-      <c r="AZ14" s="4">
-        <v>5</v>
-      </c>
-      <c r="BA14" s="4">
-        <v>5</v>
-      </c>
-      <c r="BB14" s="4">
-        <v>5</v>
-      </c>
-      <c r="BC14" s="4">
-        <v>5</v>
-      </c>
-      <c r="BD14" s="4">
-        <v>5</v>
-      </c>
-      <c r="BE14" s="4">
-        <v>5</v>
-      </c>
-      <c r="BF14" s="4">
-        <v>5</v>
-      </c>
-      <c r="BG14" s="4">
-        <v>5</v>
-      </c>
-      <c r="BH14" s="4">
-        <v>5</v>
-      </c>
-      <c r="BI14" s="4">
-        <v>5</v>
-      </c>
-      <c r="BJ14" s="4">
-        <v>5</v>
-      </c>
-      <c r="BK14" s="4">
-        <v>5</v>
-      </c>
-      <c r="BL14" s="4">
-        <v>5</v>
-      </c>
-      <c r="BM14" s="4">
-        <v>5</v>
-      </c>
-      <c r="BN14" s="4">
-        <v>5</v>
-      </c>
-      <c r="BO14" s="4">
-        <v>1</v>
-      </c>
-      <c r="BP14" s="4">
-        <v>1</v>
-      </c>
-      <c r="BQ14" s="4">
-        <v>1</v>
-      </c>
-      <c r="BR14" s="4">
-        <v>1</v>
-      </c>
-      <c r="BS14" s="4">
-        <v>1</v>
-      </c>
-      <c r="BT14" s="4">
-        <v>1</v>
-      </c>
-      <c r="BU14" s="4">
-        <v>1</v>
-      </c>
-      <c r="BV14" s="4">
-        <v>1</v>
-      </c>
-      <c r="BW14" s="4">
-        <v>1</v>
-      </c>
-      <c r="BX14" s="4">
-        <v>1</v>
-      </c>
-      <c r="BY14" s="4">
-        <v>6</v>
-      </c>
-      <c r="BZ14" s="4">
-        <v>6</v>
-      </c>
-      <c r="CA14" s="4">
-        <v>6</v>
-      </c>
-      <c r="CB14" s="4">
-        <v>6</v>
-      </c>
-      <c r="CC14" s="4">
-        <v>6</v>
-      </c>
-      <c r="CD14" s="4">
-        <v>6</v>
-      </c>
-      <c r="CE14" s="4">
-        <v>6</v>
-      </c>
-      <c r="CF14" s="4">
-        <v>6</v>
-      </c>
-      <c r="CG14" s="4">
-        <v>6</v>
-      </c>
-      <c r="CH14" s="4">
-        <v>6</v>
-      </c>
-      <c r="CI14" s="4">
-        <v>6</v>
-      </c>
-      <c r="CJ14" s="4">
-        <v>6</v>
-      </c>
-      <c r="CK14" s="4">
-        <v>6</v>
-      </c>
-      <c r="CL14" s="4">
-        <v>6</v>
-      </c>
-      <c r="CM14" s="4">
-        <v>6</v>
-      </c>
-      <c r="CN14" s="4">
-        <v>6</v>
-      </c>
-      <c r="CO14" s="4">
-        <v>7</v>
-      </c>
-      <c r="CP14" s="4">
-        <v>7</v>
-      </c>
-      <c r="CQ14" s="4">
-        <v>7</v>
-      </c>
-      <c r="CR14" s="4">
-        <v>7</v>
-      </c>
-      <c r="CS14" s="4">
-        <v>7</v>
-      </c>
-      <c r="CT14" s="4">
-        <v>7</v>
-      </c>
-      <c r="CU14" s="4">
-        <v>7</v>
-      </c>
-      <c r="CV14" s="4">
-        <v>7</v>
-      </c>
-      <c r="CW14" s="4">
-        <v>8</v>
-      </c>
-      <c r="CX14" s="4">
-        <v>8</v>
-      </c>
-      <c r="CY14" s="4">
-        <v>9</v>
-      </c>
-      <c r="CZ14" s="4">
-        <v>9</v>
-      </c>
-      <c r="DA14" s="4">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="15" spans="2:105" x14ac:dyDescent="0.25">
+        <v>78</v>
+      </c>
+      <c r="AB14" s="7"/>
+      <c r="AC14" s="7"/>
+    </row>
+    <row r="15" spans="2:107" x14ac:dyDescent="0.25">
       <c r="B15" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="AB15" s="7"/>
-      <c r="AC15" s="7"/>
-    </row>
-    <row r="16" spans="2:105" x14ac:dyDescent="0.25">
-      <c r="B16" s="6" t="s">
-        <v>195</v>
-      </c>
-      <c r="O16">
-        <v>1</v>
-      </c>
-      <c r="P16">
-        <v>1</v>
-      </c>
-      <c r="Q16">
-        <v>1</v>
-      </c>
-      <c r="R16">
-        <v>1</v>
-      </c>
-      <c r="S16">
-        <v>1</v>
-      </c>
-      <c r="T16">
-        <v>1</v>
-      </c>
-      <c r="U16">
-        <v>1</v>
-      </c>
-      <c r="V16">
-        <v>1</v>
-      </c>
-      <c r="W16">
-        <v>1</v>
-      </c>
-      <c r="X16">
-        <v>1</v>
-      </c>
-      <c r="Y16">
-        <v>1</v>
-      </c>
-      <c r="Z16">
-        <v>1</v>
-      </c>
-      <c r="CY16" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B20" t="s">
-        <v>64</v>
+        <v>192</v>
+      </c>
+      <c r="O15">
+        <v>1</v>
+      </c>
+      <c r="P15">
+        <v>1</v>
+      </c>
+      <c r="Q15">
+        <v>1</v>
+      </c>
+      <c r="R15">
+        <v>1</v>
+      </c>
+      <c r="S15">
+        <v>1</v>
+      </c>
+      <c r="T15">
+        <v>1</v>
+      </c>
+      <c r="U15">
+        <v>1</v>
+      </c>
+      <c r="V15">
+        <v>1</v>
+      </c>
+      <c r="W15">
+        <v>1</v>
+      </c>
+      <c r="X15">
+        <v>1</v>
+      </c>
+      <c r="Y15">
+        <v>1</v>
+      </c>
+      <c r="Z15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="24" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="25" spans="2:2" x14ac:dyDescent="0.25">
@@ -4370,22 +4119,17 @@
     </row>
     <row r="26" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
-        <v>69</v>
+        <v>110</v>
       </c>
     </row>
     <row r="27" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
-        <v>111</v>
+        <v>130</v>
       </c>
     </row>
     <row r="28" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="29" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B29" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
   </sheetData>
@@ -4409,7 +4153,7 @@
         <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -4417,7 +4161,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
     </row>
   </sheetData>
@@ -4637,10 +4381,10 @@
         <v>8</v>
       </c>
       <c r="E10" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="F10" s="1" t="s">
         <v>66</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -4911,16 +4655,16 @@
         <v>4</v>
       </c>
       <c r="C26" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D26" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
@@ -4928,19 +4672,19 @@
         <v>26</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D27" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E27" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F27" s="1" t="s">
         <v>71</v>
-      </c>
-      <c r="F27" s="1" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
@@ -4948,19 +4692,19 @@
         <v>27</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D28" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
@@ -4968,19 +4712,19 @@
         <v>28</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="D29" s="1" t="s">
         <v>7</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
@@ -4988,19 +4732,19 @@
         <v>29</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="D30" s="1" t="s">
         <v>7</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
@@ -5008,19 +4752,19 @@
         <v>30</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D31" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E31" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="F31" s="1" t="s">
         <v>84</v>
-      </c>
-      <c r="F31" s="1" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
@@ -5028,19 +4772,19 @@
         <v>31</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D32" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
@@ -5048,19 +4792,19 @@
         <v>32</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D33" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
@@ -5068,19 +4812,19 @@
         <v>33</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D34" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
@@ -5088,19 +4832,19 @@
         <v>34</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D35" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
@@ -5108,19 +4852,19 @@
         <v>35</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D36" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
@@ -5128,19 +4872,19 @@
         <v>36</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D37" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
@@ -5148,19 +4892,19 @@
         <v>37</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D38" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
@@ -5168,19 +4912,19 @@
         <v>38</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D39" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
@@ -5188,19 +4932,19 @@
         <v>39</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D40" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
@@ -5208,19 +4952,19 @@
         <v>40</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D41" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E41" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="F41" s="1" t="s">
         <v>105</v>
-      </c>
-      <c r="F41" s="1" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
@@ -5228,19 +4972,19 @@
         <v>41</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D42" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
@@ -5248,19 +4992,19 @@
         <v>42</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D43" s="1" t="s">
         <v>7</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
@@ -5268,19 +5012,19 @@
         <v>43</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D44" s="1" t="s">
         <v>7</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
@@ -5288,19 +5032,19 @@
         <v>44</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D45" s="1" t="s">
         <v>7</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
@@ -5308,19 +5052,19 @@
         <v>45</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D46" s="1" t="s">
         <v>7</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
@@ -5328,19 +5072,19 @@
         <v>46</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D47" s="1" t="s">
         <v>7</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
@@ -5348,19 +5092,19 @@
         <v>47</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D48" s="1" t="s">
         <v>7</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
@@ -5368,19 +5112,19 @@
         <v>48</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D49" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
@@ -5388,19 +5132,19 @@
         <v>49</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D50" s="1" t="s">
         <v>7</v>
       </c>
       <c r="E50" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="F50" s="1" t="s">
         <v>133</v>
-      </c>
-      <c r="F50" s="1" t="s">
-        <v>134</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
@@ -5408,19 +5152,19 @@
         <v>50</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D51" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F51" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
@@ -5428,19 +5172,19 @@
         <v>51</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D52" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
@@ -5448,19 +5192,19 @@
         <v>52</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D53" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E53" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="F53" s="1" t="s">
         <v>143</v>
-      </c>
-      <c r="F53" s="1" t="s">
-        <v>144</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
@@ -5468,19 +5212,19 @@
         <v>53</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D54" s="1" t="s">
         <v>7</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F54" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
@@ -5488,19 +5232,19 @@
         <v>54</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D55" s="1" t="s">
         <v>7</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="F55" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
@@ -5508,19 +5252,19 @@
         <v>55</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D56" s="1" t="s">
         <v>7</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="F56" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
@@ -5528,19 +5272,19 @@
         <v>56</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D57" s="1" t="s">
         <v>7</v>
       </c>
       <c r="E57" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="F57" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
@@ -5548,19 +5292,19 @@
         <v>57</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D58" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="F58" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
@@ -5568,19 +5312,19 @@
         <v>58</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D59" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="F59" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
@@ -5588,19 +5332,19 @@
         <v>59</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D60" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="F60" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
@@ -5608,19 +5352,19 @@
         <v>60</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C61" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D61" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="F61" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
@@ -5628,19 +5372,19 @@
         <v>61</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C62" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D62" s="1" t="s">
         <v>7</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="F62" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
@@ -5648,19 +5392,19 @@
         <v>62</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C63" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D63" s="1" t="s">
         <v>7</v>
       </c>
       <c r="E63" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="F63" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
@@ -5668,19 +5412,19 @@
         <v>63</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C64" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D64" s="1" t="s">
         <v>7</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="F64" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
@@ -5688,19 +5432,19 @@
         <v>64</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C65" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D65" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E65" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="F65" s="1" t="s">
         <v>178</v>
-      </c>
-      <c r="F65" s="1" t="s">
-        <v>179</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
@@ -5708,16 +5452,16 @@
         <v>65</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="C66" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="D66" s="1" t="s">
         <v>7</v>
       </c>
       <c r="E66" s="1" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
@@ -5725,10 +5469,10 @@
         <v>66</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="C67" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="D67" s="1" t="s">
         <v>7</v>
@@ -5739,10 +5483,10 @@
         <v>67</v>
       </c>
       <c r="B68" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="C68" t="s">
         <v>183</v>
-      </c>
-      <c r="C68" t="s">
-        <v>186</v>
       </c>
       <c r="D68" s="1" t="s">
         <v>7</v>
@@ -5753,10 +5497,10 @@
         <v>68</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="C69" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="D69" s="1" t="s">
         <v>7</v>
@@ -5767,10 +5511,10 @@
         <v>69</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="C70" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="D70" s="1" t="s">
         <v>7</v>
@@ -5781,10 +5525,10 @@
         <v>70</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="C71" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="D71" s="1" t="s">
         <v>8</v>
@@ -5795,10 +5539,10 @@
         <v>71</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="C72" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="D72" s="1" t="s">
         <v>8</v>
@@ -5809,10 +5553,10 @@
         <v>72</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="C73" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="D73" s="1" t="s">
         <v>8</v>
@@ -5823,10 +5567,10 @@
         <v>73</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="C74" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="D74" s="1" t="s">
         <v>8</v>
@@ -5837,10 +5581,10 @@
         <v>74</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="C75" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="D75" s="1" t="s">
         <v>8</v>
@@ -5867,7 +5611,7 @@
         <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -5875,7 +5619,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -5883,7 +5627,7 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -5891,7 +5635,7 @@
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
   </sheetData>
@@ -5901,10 +5645,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25CB833E-39AA-47F0-B506-E40379BB6129}">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5914,7 +5658,7 @@
         <v>1</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>181</v>
+        <v>202</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -5922,7 +5666,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>182</v>
+        <v>203</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -5930,7 +5674,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>62</v>
+        <v>204</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -5946,10 +5690,10 @@
         <v>5</v>
       </c>
       <c r="B5" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="C5" t="s">
         <v>76</v>
-      </c>
-      <c r="C5" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -5957,14 +5701,40 @@
         <v>6</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>204</v>
+        <v>209</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B7" s="8"/>
+      <c r="A7">
+        <v>7</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>8</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>207</v>
+      </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B9" s="8"/>
+      <c r="A9">
+        <v>9</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>10</v>
+      </c>
+      <c r="B10" t="s">
+        <v>206</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6002,7 +5772,7 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -6010,7 +5780,7 @@
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -6018,7 +5788,7 @@
         <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -6026,7 +5796,7 @@
         <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -6034,7 +5804,7 @@
         <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -6042,7 +5812,7 @@
         <v>8</v>
       </c>
       <c r="B8" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -6050,7 +5820,7 @@
         <v>9</v>
       </c>
       <c r="B9" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -6058,7 +5828,7 @@
         <v>10</v>
       </c>
       <c r="B10" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -6066,7 +5836,7 @@
         <v>11</v>
       </c>
       <c r="B11" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -6074,7 +5844,7 @@
         <v>12</v>
       </c>
       <c r="B12" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: Added some more features. The comparison of single-cell vs bulk works, but needs more figures and work on cortex2
</commit_message>
<xml_diff>
--- a/DesignMatrix.xlsx
+++ b/DesignMatrix.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58618146-0CAE-44F7-A3BE-C20F3A5A0687}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8A4F332-0107-4D06-BB25-857B66E35D55}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DesignMatrix" sheetId="2" r:id="rId1"/>
@@ -96,9 +96,6 @@
     <t>ENCBS495KDC</t>
   </si>
   <si>
-    <t>ENCBS714KQF</t>
-  </si>
-  <si>
     <t>CD19%2b%20B%20Cells%20%28pluriselect%29%2c%20donor090309%2c%20donation1.RDhi10007.12189-129B2.hg19.nobarcode.fq</t>
   </si>
   <si>
@@ -679,6 +676,9 @@
   </si>
   <si>
     <t>Pooled single-cell, Cord blood, Human Cell Atlas</t>
+  </si>
+  <si>
+    <t>ENCBS714KQF, ENCFF088DIY</t>
   </si>
 </sst>
 </file>
@@ -1067,8 +1067,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F369D9C3-2B00-4B3E-B4DE-89D514952C05}">
   <dimension ref="B2:DC28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J16" sqref="J16"/>
+    <sheetView topLeftCell="X1" workbookViewId="0">
+      <selection activeCell="BT11" sqref="BT11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1089,18 +1089,18 @@
         <v>4</v>
       </c>
       <c r="AB2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="BO2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="BY2" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="3" spans="2:107" x14ac:dyDescent="0.25">
       <c r="B3" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C3" s="3">
         <v>1</v>
@@ -1420,7 +1420,7 @@
     </row>
     <row r="4" spans="2:107" x14ac:dyDescent="0.25">
       <c r="B4" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C4" s="4">
         <v>2</v>
@@ -1740,7 +1740,7 @@
     </row>
     <row r="5" spans="2:107" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C5" s="4">
         <v>1</v>
@@ -2060,7 +2060,7 @@
     </row>
     <row r="6" spans="2:107" x14ac:dyDescent="0.25">
       <c r="B6" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C6" s="4">
         <v>1</v>
@@ -2380,7 +2380,7 @@
     </row>
     <row r="7" spans="2:107" x14ac:dyDescent="0.25">
       <c r="B7" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C7" s="4"/>
       <c r="D7" s="4"/>
@@ -2514,7 +2514,7 @@
     </row>
     <row r="8" spans="2:107" x14ac:dyDescent="0.25">
       <c r="B8" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C8" s="4">
         <v>2</v>
@@ -2674,7 +2674,7 @@
     </row>
     <row r="9" spans="2:107" x14ac:dyDescent="0.25">
       <c r="B9" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C9" s="4">
         <v>1</v>
@@ -2994,7 +2994,7 @@
     </row>
     <row r="10" spans="2:107" x14ac:dyDescent="0.25">
       <c r="B10" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C10" s="4">
         <v>0</v>
@@ -3314,7 +3314,7 @@
     </row>
     <row r="11" spans="2:107" x14ac:dyDescent="0.25">
       <c r="B11" s="3" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C11" s="4">
         <v>1</v>
@@ -3634,7 +3634,7 @@
     </row>
     <row r="12" spans="2:107" x14ac:dyDescent="0.25">
       <c r="B12" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C12" s="4">
         <v>1</v>
@@ -3930,7 +3930,7 @@
     </row>
     <row r="13" spans="2:107" x14ac:dyDescent="0.25">
       <c r="B13" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C13" s="4"/>
       <c r="D13" s="4">
@@ -4056,14 +4056,14 @@
     </row>
     <row r="14" spans="2:107" x14ac:dyDescent="0.25">
       <c r="B14" s="6" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="AB14" s="7"/>
       <c r="AC14" s="7"/>
     </row>
     <row r="15" spans="2:107" x14ac:dyDescent="0.25">
       <c r="B15" s="6" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="O15">
         <v>1</v>
@@ -4104,32 +4104,32 @@
     </row>
     <row r="19" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="24" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="25" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="26" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="27" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="28" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
   </sheetData>
@@ -4153,7 +4153,7 @@
         <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -4161,7 +4161,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
   </sheetData>
@@ -4173,8 +4173,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F75"/>
   <sheetViews>
-    <sheetView topLeftCell="A41" workbookViewId="0">
-      <selection activeCell="F61" sqref="F61"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4204,7 +4204,7 @@
         <v>3</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -4221,10 +4221,10 @@
         <v>7</v>
       </c>
       <c r="E2" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>44</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -4241,10 +4241,10 @@
         <v>7</v>
       </c>
       <c r="E3" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="F3" s="1" t="s">
         <v>53</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -4261,10 +4261,10 @@
         <v>7</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -4281,10 +4281,10 @@
         <v>7</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -4301,10 +4301,10 @@
         <v>7</v>
       </c>
       <c r="E6" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F6" s="1" t="s">
         <v>57</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -4321,10 +4321,10 @@
         <v>7</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -4341,10 +4341,10 @@
         <v>7</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -4361,10 +4361,10 @@
         <v>8</v>
       </c>
       <c r="E9" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="F9" s="1" t="s">
         <v>50</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -4381,10 +4381,10 @@
         <v>8</v>
       </c>
       <c r="E10" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="F10" s="1" t="s">
         <v>65</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -4401,10 +4401,10 @@
         <v>8</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -4421,10 +4421,10 @@
         <v>8</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -4435,16 +4435,16 @@
         <v>4</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>15</v>
+        <v>209</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -4459,10 +4459,10 @@
         <v>7</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -4478,7 +4478,7 @@
       </c>
       <c r="E15" s="1"/>
       <c r="F15" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
@@ -4494,7 +4494,7 @@
       </c>
       <c r="E16" s="1"/>
       <c r="F16" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
@@ -4509,10 +4509,10 @@
         <v>7</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
@@ -4528,7 +4528,7 @@
       </c>
       <c r="E18" s="1"/>
       <c r="F18" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
@@ -4544,7 +4544,7 @@
       </c>
       <c r="E19" s="1"/>
       <c r="F19" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
@@ -4559,10 +4559,10 @@
         <v>8</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
@@ -4578,7 +4578,7 @@
       </c>
       <c r="E21" s="1"/>
       <c r="F21" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
@@ -4594,7 +4594,7 @@
       </c>
       <c r="E22" s="1"/>
       <c r="F22" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
@@ -4609,10 +4609,10 @@
         <v>8</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
@@ -4628,7 +4628,7 @@
       </c>
       <c r="E24" s="1"/>
       <c r="F24" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
@@ -4644,7 +4644,7 @@
       </c>
       <c r="E25" s="1"/>
       <c r="F25" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
@@ -4655,16 +4655,16 @@
         <v>4</v>
       </c>
       <c r="C26" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D26" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
@@ -4672,19 +4672,19 @@
         <v>26</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D27" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E27" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="F27" s="1" t="s">
         <v>70</v>
-      </c>
-      <c r="F27" s="1" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
@@ -4692,19 +4692,19 @@
         <v>27</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D28" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
@@ -4712,19 +4712,19 @@
         <v>28</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D29" s="1" t="s">
         <v>7</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
@@ -4732,19 +4732,19 @@
         <v>29</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D30" s="1" t="s">
         <v>7</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
@@ -4752,19 +4752,19 @@
         <v>30</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D31" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E31" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="F31" s="1" t="s">
         <v>83</v>
-      </c>
-      <c r="F31" s="1" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
@@ -4772,19 +4772,19 @@
         <v>31</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D32" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
@@ -4792,19 +4792,19 @@
         <v>32</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D33" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
@@ -4812,19 +4812,19 @@
         <v>33</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D34" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
@@ -4832,19 +4832,19 @@
         <v>34</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D35" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
@@ -4852,19 +4852,19 @@
         <v>35</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D36" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
@@ -4872,19 +4872,19 @@
         <v>36</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D37" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
@@ -4892,19 +4892,19 @@
         <v>37</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D38" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
@@ -4912,19 +4912,19 @@
         <v>38</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D39" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
@@ -4932,19 +4932,19 @@
         <v>39</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D40" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
@@ -4952,19 +4952,19 @@
         <v>40</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D41" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E41" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="F41" s="1" t="s">
         <v>104</v>
-      </c>
-      <c r="F41" s="1" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
@@ -4972,19 +4972,19 @@
         <v>41</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D42" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
@@ -4992,19 +4992,19 @@
         <v>42</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D43" s="1" t="s">
         <v>7</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
@@ -5012,19 +5012,19 @@
         <v>43</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D44" s="1" t="s">
         <v>7</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
@@ -5032,19 +5032,19 @@
         <v>44</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D45" s="1" t="s">
         <v>7</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
@@ -5052,19 +5052,19 @@
         <v>45</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D46" s="1" t="s">
         <v>7</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
@@ -5072,19 +5072,19 @@
         <v>46</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D47" s="1" t="s">
         <v>7</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
@@ -5092,19 +5092,19 @@
         <v>47</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D48" s="1" t="s">
         <v>7</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
@@ -5112,19 +5112,19 @@
         <v>48</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D49" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
@@ -5132,19 +5132,19 @@
         <v>49</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D50" s="1" t="s">
         <v>7</v>
       </c>
       <c r="E50" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="F50" s="1" t="s">
         <v>132</v>
-      </c>
-      <c r="F50" s="1" t="s">
-        <v>133</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
@@ -5152,19 +5152,19 @@
         <v>50</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D51" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F51" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
@@ -5172,19 +5172,19 @@
         <v>51</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D52" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
@@ -5192,19 +5192,19 @@
         <v>52</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D53" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E53" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="F53" s="1" t="s">
         <v>142</v>
-      </c>
-      <c r="F53" s="1" t="s">
-        <v>143</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
@@ -5212,19 +5212,19 @@
         <v>53</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D54" s="1" t="s">
         <v>7</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="F54" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
@@ -5232,19 +5232,19 @@
         <v>54</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D55" s="1" t="s">
         <v>7</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="F55" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
@@ -5252,19 +5252,19 @@
         <v>55</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D56" s="1" t="s">
         <v>7</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="F56" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
@@ -5272,19 +5272,19 @@
         <v>56</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D57" s="1" t="s">
         <v>7</v>
       </c>
       <c r="E57" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="F57" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
@@ -5292,19 +5292,19 @@
         <v>57</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D58" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="F58" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
@@ -5312,19 +5312,19 @@
         <v>58</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D59" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="F59" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
@@ -5332,19 +5332,19 @@
         <v>59</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D60" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="F60" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
@@ -5352,19 +5352,19 @@
         <v>60</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C61" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D61" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="F61" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
@@ -5372,19 +5372,19 @@
         <v>61</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C62" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D62" s="1" t="s">
         <v>7</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="F62" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
@@ -5392,19 +5392,19 @@
         <v>62</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C63" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D63" s="1" t="s">
         <v>7</v>
       </c>
       <c r="E63" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="F63" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
@@ -5412,19 +5412,19 @@
         <v>63</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C64" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D64" s="1" t="s">
         <v>7</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="F64" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
@@ -5432,19 +5432,19 @@
         <v>64</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C65" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D65" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E65" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="F65" s="1" t="s">
         <v>177</v>
-      </c>
-      <c r="F65" s="1" t="s">
-        <v>178</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
@@ -5452,16 +5452,16 @@
         <v>65</v>
       </c>
       <c r="B66" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="C66" t="s">
         <v>180</v>
-      </c>
-      <c r="C66" t="s">
-        <v>181</v>
       </c>
       <c r="D66" s="1" t="s">
         <v>7</v>
       </c>
       <c r="E66" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
@@ -5469,10 +5469,10 @@
         <v>66</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C67" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D67" s="1" t="s">
         <v>7</v>
@@ -5483,10 +5483,10 @@
         <v>67</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C68" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D68" s="1" t="s">
         <v>7</v>
@@ -5497,10 +5497,10 @@
         <v>68</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C69" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D69" s="1" t="s">
         <v>7</v>
@@ -5511,10 +5511,10 @@
         <v>69</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C70" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D70" s="1" t="s">
         <v>7</v>
@@ -5525,10 +5525,10 @@
         <v>70</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C71" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D71" s="1" t="s">
         <v>8</v>
@@ -5539,10 +5539,10 @@
         <v>71</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C72" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D72" s="1" t="s">
         <v>8</v>
@@ -5553,10 +5553,10 @@
         <v>72</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C73" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D73" s="1" t="s">
         <v>8</v>
@@ -5567,10 +5567,10 @@
         <v>73</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C74" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D74" s="1" t="s">
         <v>8</v>
@@ -5581,10 +5581,10 @@
         <v>74</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C75" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D75" s="1" t="s">
         <v>8</v>
@@ -5611,7 +5611,7 @@
         <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -5619,7 +5619,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -5627,7 +5627,7 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -5635,7 +5635,7 @@
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
   </sheetData>
@@ -5648,7 +5648,7 @@
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5658,7 +5658,7 @@
         <v>1</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -5666,7 +5666,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -5674,7 +5674,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -5682,7 +5682,7 @@
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -5690,10 +5690,10 @@
         <v>5</v>
       </c>
       <c r="B5" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="C5" t="s">
         <v>75</v>
-      </c>
-      <c r="C5" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -5701,7 +5701,7 @@
         <v>6</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -5709,7 +5709,7 @@
         <v>7</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -5717,7 +5717,7 @@
         <v>8</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -5725,7 +5725,7 @@
         <v>9</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -5733,7 +5733,7 @@
         <v>10</v>
       </c>
       <c r="B10" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
   </sheetData>
@@ -5756,7 +5756,7 @@
         <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -5764,7 +5764,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -5772,7 +5772,7 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -5780,7 +5780,7 @@
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -5788,7 +5788,7 @@
         <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -5796,7 +5796,7 @@
         <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -5804,7 +5804,7 @@
         <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -5812,7 +5812,7 @@
         <v>8</v>
       </c>
       <c r="B8" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -5820,7 +5820,7 @@
         <v>9</v>
       </c>
       <c r="B9" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -5828,7 +5828,7 @@
         <v>10</v>
       </c>
       <c r="B10" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -5836,7 +5836,7 @@
         <v>11</v>
       </c>
       <c r="B11" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -5844,7 +5844,7 @@
         <v>12</v>
       </c>
       <c r="B12" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix: cleaned up the design matrix, removing unused rows (except for bulk/single-cell, which may be useful for separating labs)
</commit_message>
<xml_diff>
--- a/DesignMatrix.xlsx
+++ b/DesignMatrix.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8A4F332-0107-4D06-BB25-857B66E35D55}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEFF38A3-D00B-4A1E-BF3B-57C38EBE6CF5}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DesignMatrix" sheetId="2" r:id="rId1"/>
@@ -30,26 +30,8 @@
 </workbook>
 </file>
 
-<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
-  <authors>
-    <author>tc={700C9106-279A-4568-A95C-D4F66DD031F0}</author>
-  </authors>
-  <commentList>
-    <comment ref="CY9" authorId="0" shapeId="0" xr:uid="{700C9106-279A-4568-A95C-D4F66DD031F0}">
-      <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    A bit unclear exactly which type of CD4 memory T cell this is</t>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="391" uniqueCount="210">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="380" uniqueCount="199">
   <si>
     <t>Sample index</t>
   </si>
@@ -144,24 +126,15 @@
     <t>Bulk=1</t>
   </si>
   <si>
-    <t>Expanded (yes==1)</t>
-  </si>
-  <si>
     <t>B cells, 3 samples from the same patient, FANTOM5</t>
   </si>
   <si>
     <t>T cells, 3 samples from the same patient, FANTOM5</t>
   </si>
   <si>
-    <t>RNA-Seq method</t>
-  </si>
-  <si>
     <t>Sub Cell type</t>
   </si>
   <si>
-    <t>Poly-A</t>
-  </si>
-  <si>
     <t>Original files</t>
   </si>
   <si>
@@ -237,9 +210,6 @@
     <t>ENCBS424MFE</t>
   </si>
   <si>
-    <t>Not run:</t>
-  </si>
-  <si>
     <t>male adult (21 year) CD4-positive, alpha-beta T primary cell, John Stamatoyannopoulos</t>
   </si>
   <si>
@@ -249,12 +219,6 @@
     <t>ENCFF249TVM-1.fastq.gz, ENCFF570NFU-2.fastq.gz</t>
   </si>
   <si>
-    <t>Additional info:</t>
-  </si>
-  <si>
-    <t>There are also 6 samples in ENCODE that are identical to sample 2-7, except that they are rRNA-depleted before running polyA RNA-Seq. We did not include them.</t>
-  </si>
-  <si>
     <t>BLUEPRINT</t>
   </si>
   <si>
@@ -282,9 +246,6 @@
     <t>CD4+ T cell</t>
   </si>
   <si>
-    <t>rRNA depletion</t>
-  </si>
-  <si>
     <t>CD38-negative naive B cell</t>
   </si>
   <si>
@@ -378,9 +339,6 @@
     <t>CD3-, CD4+, CD8+ T cell</t>
   </si>
   <si>
-    <t>Skipped BLUEPRINT Dataset EGAD00001002287, acute lymphocytic leukemia</t>
-  </si>
-  <si>
     <t>141030_SN935_0211_B_C5R24ACXX_ACAGTG_1_read1.fastq.gz, 141030_SN935_0211_B_C5R24ACXX_ACAGTG_1_read2.fastq.gz</t>
   </si>
   <si>
@@ -438,9 +396,6 @@
     <t>Effector memory CD8+ T cell</t>
   </si>
   <si>
-    <t>Skipped BLUEPRINT Dataset EGAD00001002321, since it contains NK cells only</t>
-  </si>
-  <si>
     <t>EGAD00001002347</t>
   </si>
   <si>
@@ -495,9 +450,6 @@
     <t>Unswitched memory B cell</t>
   </si>
   <si>
-    <t>Skipped BLUEPRINT EGAD00001002426, prolymphocytic leukemia</t>
-  </si>
-  <si>
     <t>RNA-Seq for germinal center B cell, on genome GRCh38</t>
   </si>
   <si>
@@ -622,9 +574,6 @@
   </si>
   <si>
     <t>We don't have the fastq files for these samples</t>
-  </si>
-  <si>
-    <t>Single-stranded</t>
   </si>
   <si>
     <t>ENCFF861MLB-1.fastq.gz, ENCFF141XOX-2.fastq.gz</t>
@@ -708,7 +657,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -721,14 +670,8 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -751,32 +694,18 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1055,20 +984,12 @@
 </a:theme>
 </file>
 
-<file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
-<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <threadedComment ref="CY9" dT="2019-08-27T15:46:26.03" personId="{00000000-0000-0000-0000-000000000000}" id="{700C9106-279A-4568-A95C-D4F66DD031F0}">
-    <text>A bit unclear exactly which type of CD4 memory T cell this is</text>
-  </threadedComment>
-</ThreadedComments>
-</file>
-
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F369D9C3-2B00-4B3E-B4DE-89D514952C05}">
-  <dimension ref="B2:DC28"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F369D9C3-2B00-4B3E-B4DE-89D514952C05}">
+  <dimension ref="B2:DC10"/>
   <sheetViews>
-    <sheetView topLeftCell="X1" workbookViewId="0">
-      <selection activeCell="BT11" sqref="BT11"/>
+    <sheetView tabSelected="1" topLeftCell="AX1" workbookViewId="0">
+      <selection activeCell="CW10" sqref="CW10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1089,13 +1010,13 @@
         <v>4</v>
       </c>
       <c r="AB2" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="BO2" t="s">
-        <v>179</v>
+        <v>169</v>
       </c>
       <c r="BY2" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
     </row>
     <row r="3" spans="2:107" x14ac:dyDescent="0.25">
@@ -2380,73 +2301,99 @@
     </row>
     <row r="7" spans="2:107" x14ac:dyDescent="0.25">
       <c r="B7" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4"/>
-      <c r="G7" s="4"/>
-      <c r="H7" s="4"/>
-      <c r="I7" s="4"/>
-      <c r="J7" s="4"/>
-      <c r="K7" s="4"/>
-      <c r="L7" s="4"/>
-      <c r="M7" s="4"/>
-      <c r="N7" s="4"/>
-      <c r="O7" s="4">
+        <v>39</v>
+      </c>
+      <c r="C7" s="4">
+        <v>2</v>
+      </c>
+      <c r="D7" s="4">
+        <v>4</v>
+      </c>
+      <c r="E7" s="4">
+        <v>4</v>
+      </c>
+      <c r="F7" s="4">
+        <v>4</v>
+      </c>
+      <c r="G7" s="4">
+        <v>5</v>
+      </c>
+      <c r="H7" s="4">
+        <v>5</v>
+      </c>
+      <c r="I7" s="4">
+        <v>5</v>
+      </c>
+      <c r="J7" s="4">
         <v>6</v>
       </c>
-      <c r="P7" s="4">
+      <c r="K7" s="4">
+        <v>2</v>
+      </c>
+      <c r="L7" s="4">
+        <v>2</v>
+      </c>
+      <c r="M7" s="4">
+        <v>2</v>
+      </c>
+      <c r="N7" s="4">
+        <v>2</v>
+      </c>
+      <c r="O7" s="5">
+        <v>1</v>
+      </c>
+      <c r="P7" s="5">
+        <v>1</v>
+      </c>
+      <c r="Q7" s="5">
+        <v>1</v>
+      </c>
+      <c r="R7" s="5">
+        <v>3</v>
+      </c>
+      <c r="S7" s="5">
+        <v>3</v>
+      </c>
+      <c r="T7" s="5">
+        <v>3</v>
+      </c>
+      <c r="U7" s="5">
+        <v>1</v>
+      </c>
+      <c r="V7" s="5">
+        <v>1</v>
+      </c>
+      <c r="W7" s="5">
+        <v>1</v>
+      </c>
+      <c r="X7" s="5">
+        <v>3</v>
+      </c>
+      <c r="Y7" s="5">
+        <v>3</v>
+      </c>
+      <c r="Z7" s="5">
+        <v>3</v>
+      </c>
+      <c r="AA7" s="5">
         <v>6</v>
       </c>
-      <c r="Q7" s="4">
-        <v>6</v>
-      </c>
-      <c r="R7" s="4">
-        <v>6</v>
-      </c>
-      <c r="S7" s="4">
-        <v>6</v>
-      </c>
-      <c r="T7" s="4">
-        <v>6</v>
-      </c>
-      <c r="U7" s="4">
-        <v>6</v>
-      </c>
-      <c r="V7" s="4">
-        <v>6</v>
-      </c>
-      <c r="W7" s="4">
-        <v>6</v>
-      </c>
-      <c r="X7" s="4">
-        <v>6</v>
-      </c>
-      <c r="Y7" s="4">
-        <v>6</v>
-      </c>
-      <c r="Z7" s="4">
-        <v>6</v>
-      </c>
-      <c r="AA7" s="4"/>
-      <c r="AB7" s="4"/>
-      <c r="AC7" s="4"/>
-      <c r="AD7" s="4"/>
-      <c r="AE7" s="4"/>
-      <c r="AF7" s="4"/>
-      <c r="AG7" s="4"/>
-      <c r="AH7" s="4"/>
-      <c r="AI7" s="4"/>
-      <c r="AJ7" s="4"/>
-      <c r="AK7" s="4"/>
-      <c r="AL7" s="4"/>
-      <c r="AM7" s="4"/>
-      <c r="AN7" s="4"/>
-      <c r="AO7" s="4"/>
-      <c r="AP7" s="4"/>
-      <c r="AQ7" s="4"/>
+      <c r="AB7" s="5"/>
+      <c r="AC7" s="5"/>
+      <c r="AD7" s="5"/>
+      <c r="AE7" s="5"/>
+      <c r="AF7" s="5"/>
+      <c r="AG7" s="5"/>
+      <c r="AH7" s="5"/>
+      <c r="AI7" s="5"/>
+      <c r="AJ7" s="5"/>
+      <c r="AK7" s="5"/>
+      <c r="AL7" s="5"/>
+      <c r="AM7" s="5"/>
+      <c r="AN7" s="5"/>
+      <c r="AO7" s="5"/>
+      <c r="AP7" s="5"/>
+      <c r="AQ7" s="5"/>
       <c r="AR7" s="4"/>
       <c r="AS7" s="4"/>
       <c r="AT7" s="4"/>
@@ -2514,167 +2461,327 @@
     </row>
     <row r="8" spans="2:107" x14ac:dyDescent="0.25">
       <c r="B8" s="3" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="C8" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D8" s="4">
+        <v>1</v>
+      </c>
+      <c r="E8" s="4">
+        <v>1</v>
+      </c>
+      <c r="F8" s="4">
+        <v>1</v>
+      </c>
+      <c r="G8" s="4">
+        <v>1</v>
+      </c>
+      <c r="H8" s="4">
+        <v>1</v>
+      </c>
+      <c r="I8" s="4">
+        <v>1</v>
+      </c>
+      <c r="J8" s="4">
+        <v>2</v>
+      </c>
+      <c r="K8" s="4">
+        <v>3</v>
+      </c>
+      <c r="L8" s="4">
+        <v>1</v>
+      </c>
+      <c r="M8" s="4">
+        <v>1</v>
+      </c>
+      <c r="N8" s="4">
+        <v>2</v>
+      </c>
+      <c r="O8" s="4">
+        <v>1</v>
+      </c>
+      <c r="P8" s="4">
+        <v>1</v>
+      </c>
+      <c r="Q8" s="4">
+        <v>1</v>
+      </c>
+      <c r="R8" s="4">
+        <v>1</v>
+      </c>
+      <c r="S8" s="4">
+        <v>1</v>
+      </c>
+      <c r="T8" s="4">
+        <v>1</v>
+      </c>
+      <c r="U8" s="4">
+        <v>1</v>
+      </c>
+      <c r="V8" s="4">
+        <v>1</v>
+      </c>
+      <c r="W8" s="4">
+        <v>1</v>
+      </c>
+      <c r="X8" s="4">
+        <v>1</v>
+      </c>
+      <c r="Y8" s="4">
+        <v>1</v>
+      </c>
+      <c r="Z8" s="4">
+        <v>1</v>
+      </c>
+      <c r="AA8" s="4">
+        <v>3</v>
+      </c>
+      <c r="AB8" s="4">
+        <v>2</v>
+      </c>
+      <c r="AC8" s="4">
+        <v>2</v>
+      </c>
+      <c r="AD8" s="4">
+        <v>1</v>
+      </c>
+      <c r="AE8" s="4">
+        <v>1</v>
+      </c>
+      <c r="AF8" s="4">
+        <v>3</v>
+      </c>
+      <c r="AG8" s="4">
+        <v>3</v>
+      </c>
+      <c r="AH8" s="4">
+        <v>3</v>
+      </c>
+      <c r="AI8" s="4">
+        <v>3</v>
+      </c>
+      <c r="AJ8" s="4">
+        <v>3</v>
+      </c>
+      <c r="AK8" s="4">
+        <v>3</v>
+      </c>
+      <c r="AL8" s="4">
+        <v>3</v>
+      </c>
+      <c r="AM8" s="4">
+        <v>3</v>
+      </c>
+      <c r="AN8" s="4">
+        <v>3</v>
+      </c>
+      <c r="AO8" s="4">
+        <v>3</v>
+      </c>
+      <c r="AP8" s="4">
+        <v>2</v>
+      </c>
+      <c r="AQ8" s="4">
         <v>4</v>
       </c>
-      <c r="E8" s="4">
-        <v>4</v>
-      </c>
-      <c r="F8" s="4">
-        <v>4</v>
-      </c>
-      <c r="G8" s="4">
+      <c r="AR8" s="4">
+        <v>1</v>
+      </c>
+      <c r="AS8" s="4">
+        <v>1</v>
+      </c>
+      <c r="AT8" s="4">
+        <v>1</v>
+      </c>
+      <c r="AU8" s="4">
+        <v>1</v>
+      </c>
+      <c r="AV8" s="4">
+        <v>1</v>
+      </c>
+      <c r="AW8" s="4">
+        <v>1</v>
+      </c>
+      <c r="AX8" s="4">
         <v>5</v>
       </c>
-      <c r="H8" s="4">
+      <c r="AY8" s="4">
+        <v>6</v>
+      </c>
+      <c r="AZ8" s="4">
+        <v>7</v>
+      </c>
+      <c r="BA8" s="4">
+        <v>7</v>
+      </c>
+      <c r="BB8" s="4">
+        <v>8</v>
+      </c>
+      <c r="BC8" s="4">
+        <v>9</v>
+      </c>
+      <c r="BD8" s="4">
+        <v>1</v>
+      </c>
+      <c r="BE8" s="4">
+        <v>1</v>
+      </c>
+      <c r="BF8" s="4">
+        <v>1</v>
+      </c>
+      <c r="BG8" s="4">
         <v>5</v>
       </c>
-      <c r="I8" s="4">
+      <c r="BH8" s="4">
         <v>5</v>
       </c>
-      <c r="J8" s="4">
-        <v>6</v>
-      </c>
-      <c r="K8" s="4">
-        <v>2</v>
-      </c>
-      <c r="L8" s="4">
-        <v>2</v>
-      </c>
-      <c r="M8" s="4">
-        <v>2</v>
-      </c>
-      <c r="N8" s="4">
-        <v>2</v>
-      </c>
-      <c r="O8" s="5">
-        <v>1</v>
-      </c>
-      <c r="P8" s="5">
-        <v>1</v>
-      </c>
-      <c r="Q8" s="5">
-        <v>1</v>
-      </c>
-      <c r="R8" s="5">
-        <v>3</v>
-      </c>
-      <c r="S8" s="5">
-        <v>3</v>
-      </c>
-      <c r="T8" s="5">
-        <v>3</v>
-      </c>
-      <c r="U8" s="5">
-        <v>1</v>
-      </c>
-      <c r="V8" s="5">
-        <v>1</v>
-      </c>
-      <c r="W8" s="5">
-        <v>1</v>
-      </c>
-      <c r="X8" s="5">
-        <v>3</v>
-      </c>
-      <c r="Y8" s="5">
-        <v>3</v>
-      </c>
-      <c r="Z8" s="5">
-        <v>3</v>
-      </c>
-      <c r="AA8" s="5">
-        <v>6</v>
-      </c>
-      <c r="AB8" s="5"/>
-      <c r="AC8" s="5"/>
-      <c r="AD8" s="5"/>
-      <c r="AE8" s="5"/>
-      <c r="AF8" s="5"/>
-      <c r="AG8" s="5"/>
-      <c r="AH8" s="5"/>
-      <c r="AI8" s="5"/>
-      <c r="AJ8" s="5"/>
-      <c r="AK8" s="5"/>
-      <c r="AL8" s="5"/>
-      <c r="AM8" s="5"/>
-      <c r="AN8" s="5"/>
-      <c r="AO8" s="5"/>
-      <c r="AP8" s="5"/>
-      <c r="AQ8" s="5"/>
-      <c r="AR8" s="4"/>
-      <c r="AS8" s="4"/>
-      <c r="AT8" s="4"/>
-      <c r="AU8" s="4"/>
-      <c r="AV8" s="4"/>
-      <c r="AW8" s="4"/>
-      <c r="AX8" s="4"/>
-      <c r="AY8" s="4"/>
-      <c r="AZ8" s="4"/>
-      <c r="BA8" s="4"/>
-      <c r="BB8" s="4"/>
-      <c r="BC8" s="4"/>
-      <c r="BD8" s="4"/>
-      <c r="BE8" s="4"/>
-      <c r="BF8" s="4"/>
-      <c r="BG8" s="4"/>
-      <c r="BH8" s="4"/>
-      <c r="BI8" s="4"/>
-      <c r="BJ8" s="4"/>
-      <c r="BK8" s="4"/>
-      <c r="BL8" s="4"/>
-      <c r="BM8" s="4"/>
-      <c r="BN8" s="4"/>
-      <c r="BO8" s="4"/>
-      <c r="BP8" s="4"/>
-      <c r="BQ8" s="4"/>
-      <c r="BR8" s="4"/>
-      <c r="BS8" s="4"/>
-      <c r="BT8" s="4"/>
-      <c r="BU8" s="4"/>
-      <c r="BV8" s="4"/>
-      <c r="BW8" s="4"/>
-      <c r="BX8" s="4"/>
-      <c r="BY8" s="4"/>
-      <c r="BZ8" s="4"/>
-      <c r="CA8" s="4"/>
-      <c r="CB8" s="4"/>
-      <c r="CC8" s="4"/>
-      <c r="CD8" s="4"/>
-      <c r="CE8" s="4"/>
-      <c r="CF8" s="4"/>
-      <c r="CG8" s="4"/>
-      <c r="CH8" s="4"/>
-      <c r="CI8" s="4"/>
-      <c r="CJ8" s="4"/>
-      <c r="CK8" s="4"/>
-      <c r="CL8" s="4"/>
-      <c r="CM8" s="4"/>
-      <c r="CN8" s="4"/>
-      <c r="CO8" s="4"/>
-      <c r="CP8" s="4"/>
-      <c r="CQ8" s="4"/>
-      <c r="CR8" s="4"/>
-      <c r="CS8" s="4"/>
-      <c r="CT8" s="4"/>
-      <c r="CU8" s="4"/>
-      <c r="CV8" s="4"/>
-      <c r="CW8" s="4"/>
-      <c r="CX8" s="4"/>
-      <c r="CY8" s="4"/>
-      <c r="CZ8" s="4"/>
-      <c r="DA8" s="4"/>
-      <c r="DB8" s="4"/>
-      <c r="DC8" s="4"/>
+      <c r="BI8" s="4">
+        <v>10</v>
+      </c>
+      <c r="BJ8" s="4">
+        <v>10</v>
+      </c>
+      <c r="BK8" s="4">
+        <v>11</v>
+      </c>
+      <c r="BL8" s="4">
+        <v>11</v>
+      </c>
+      <c r="BM8" s="4">
+        <v>11</v>
+      </c>
+      <c r="BN8" s="4">
+        <v>12</v>
+      </c>
+      <c r="BO8" s="4">
+        <v>1</v>
+      </c>
+      <c r="BP8" s="4">
+        <v>1</v>
+      </c>
+      <c r="BQ8" s="4">
+        <v>1</v>
+      </c>
+      <c r="BR8" s="4">
+        <v>1</v>
+      </c>
+      <c r="BS8" s="4">
+        <v>1</v>
+      </c>
+      <c r="BT8" s="4">
+        <v>1</v>
+      </c>
+      <c r="BU8" s="4">
+        <v>1</v>
+      </c>
+      <c r="BV8" s="4">
+        <v>1</v>
+      </c>
+      <c r="BW8" s="4">
+        <v>1</v>
+      </c>
+      <c r="BX8" s="4">
+        <v>1</v>
+      </c>
+      <c r="BY8" s="4">
+        <v>1</v>
+      </c>
+      <c r="BZ8" s="4">
+        <v>1</v>
+      </c>
+      <c r="CA8" s="4">
+        <v>1</v>
+      </c>
+      <c r="CB8" s="4">
+        <v>1</v>
+      </c>
+      <c r="CC8" s="4">
+        <v>1</v>
+      </c>
+      <c r="CD8" s="4">
+        <v>1</v>
+      </c>
+      <c r="CE8" s="4">
+        <v>1</v>
+      </c>
+      <c r="CF8" s="4">
+        <v>1</v>
+      </c>
+      <c r="CG8" s="4">
+        <v>1</v>
+      </c>
+      <c r="CH8" s="4">
+        <v>1</v>
+      </c>
+      <c r="CI8" s="4">
+        <v>1</v>
+      </c>
+      <c r="CJ8" s="4">
+        <v>1</v>
+      </c>
+      <c r="CK8" s="4">
+        <v>1</v>
+      </c>
+      <c r="CL8" s="4">
+        <v>1</v>
+      </c>
+      <c r="CM8" s="4">
+        <v>1</v>
+      </c>
+      <c r="CN8" s="4">
+        <v>1</v>
+      </c>
+      <c r="CO8" s="4">
+        <v>1</v>
+      </c>
+      <c r="CP8" s="4">
+        <v>1</v>
+      </c>
+      <c r="CQ8" s="4">
+        <v>1</v>
+      </c>
+      <c r="CR8" s="4">
+        <v>1</v>
+      </c>
+      <c r="CS8" s="4">
+        <v>1</v>
+      </c>
+      <c r="CT8" s="4">
+        <v>1</v>
+      </c>
+      <c r="CU8" s="4">
+        <v>1</v>
+      </c>
+      <c r="CV8" s="4">
+        <v>1</v>
+      </c>
+      <c r="CW8" s="4">
+        <v>1</v>
+      </c>
+      <c r="CX8" s="4">
+        <v>1</v>
+      </c>
+      <c r="CY8" s="4">
+        <v>10</v>
+      </c>
+      <c r="CZ8" s="4">
+        <v>1</v>
+      </c>
+      <c r="DA8" s="4">
+        <v>2</v>
+      </c>
+      <c r="DB8" s="4">
+        <v>1</v>
+      </c>
+      <c r="DC8" s="4">
+        <v>1</v>
+      </c>
     </row>
     <row r="9" spans="2:107" x14ac:dyDescent="0.25">
       <c r="B9" s="3" t="s">
-        <v>35</v>
+        <v>189</v>
       </c>
       <c r="C9" s="4">
         <v>1</v>
@@ -2701,13 +2808,13 @@
         <v>2</v>
       </c>
       <c r="K9" s="4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="L9" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M9" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N9" s="4">
         <v>2</v>
@@ -2731,25 +2838,25 @@
         <v>1</v>
       </c>
       <c r="U9" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="V9" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="W9" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="X9" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Y9" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Z9" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AA9" s="4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AB9" s="4">
         <v>2</v>
@@ -2764,40 +2871,40 @@
         <v>1</v>
       </c>
       <c r="AF9" s="4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AG9" s="4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AH9" s="4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AI9" s="4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AJ9" s="4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AK9" s="4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AL9" s="4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AM9" s="4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AN9" s="4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AO9" s="4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AP9" s="4">
         <v>2</v>
       </c>
       <c r="AQ9" s="4">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="AR9" s="4">
         <v>1</v>
@@ -2818,22 +2925,22 @@
         <v>1</v>
       </c>
       <c r="AX9" s="4">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="AY9" s="4">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="AZ9" s="4">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="BA9" s="4">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="BB9" s="4">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="BC9" s="4">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="BD9" s="4">
         <v>1</v>
@@ -2845,28 +2952,28 @@
         <v>1</v>
       </c>
       <c r="BG9" s="4">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="BH9" s="4">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="BI9" s="4">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="BJ9" s="4">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="BK9" s="4">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="BL9" s="4">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="BM9" s="4">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="BN9" s="4">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="BO9" s="4">
         <v>1</v>
@@ -2884,43 +2991,43 @@
         <v>1</v>
       </c>
       <c r="BT9" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="BU9" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="BV9" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="BW9" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="BX9" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="BY9" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="BZ9" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="CA9" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="CB9" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="CC9" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="CD9" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="CE9" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="CF9" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="CG9" s="4">
         <v>1</v>
@@ -2947,13 +3054,13 @@
         <v>1</v>
       </c>
       <c r="CO9" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="CP9" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="CQ9" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="CR9" s="4">
         <v>1</v>
@@ -2965,19 +3072,19 @@
         <v>1</v>
       </c>
       <c r="CU9" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="CV9" s="4">
         <v>1</v>
       </c>
       <c r="CW9" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="CX9" s="4">
         <v>1</v>
       </c>
       <c r="CY9" s="4">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="CZ9" s="4">
         <v>1</v>
@@ -2986,7 +3093,7 @@
         <v>2</v>
       </c>
       <c r="DB9" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="DC9" s="4">
         <v>1</v>
@@ -2994,1147 +3101,132 @@
     </row>
     <row r="10" spans="2:107" x14ac:dyDescent="0.25">
       <c r="B10" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="C10" s="4">
-        <v>0</v>
-      </c>
+        <v>57</v>
+      </c>
+      <c r="C10" s="4"/>
       <c r="D10" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E10" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F10" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G10" s="4">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H10" s="4">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I10" s="4">
-        <v>0</v>
-      </c>
-      <c r="J10" s="4">
-        <v>0</v>
-      </c>
-      <c r="K10" s="4">
-        <v>0</v>
-      </c>
-      <c r="L10" s="4">
-        <v>0</v>
-      </c>
-      <c r="M10" s="4">
-        <v>0</v>
-      </c>
-      <c r="N10" s="4">
-        <v>0</v>
-      </c>
-      <c r="O10" s="4">
-        <v>0</v>
-      </c>
-      <c r="P10" s="4">
-        <v>0</v>
-      </c>
-      <c r="Q10" s="4">
-        <v>0</v>
-      </c>
-      <c r="R10" s="4">
-        <v>0</v>
-      </c>
-      <c r="S10" s="4">
-        <v>0</v>
-      </c>
-      <c r="T10" s="4">
-        <v>0</v>
-      </c>
-      <c r="U10" s="4">
-        <v>0</v>
-      </c>
-      <c r="V10" s="4">
-        <v>0</v>
-      </c>
-      <c r="W10" s="4">
-        <v>0</v>
-      </c>
-      <c r="X10" s="4">
-        <v>0</v>
-      </c>
-      <c r="Y10" s="4">
-        <v>0</v>
-      </c>
-      <c r="Z10" s="4">
-        <v>0</v>
-      </c>
-      <c r="AA10" s="4">
-        <v>0</v>
-      </c>
-      <c r="AB10" s="4">
-        <v>0</v>
-      </c>
-      <c r="AC10" s="4">
-        <v>0</v>
-      </c>
-      <c r="AD10" s="4">
-        <v>0</v>
-      </c>
-      <c r="AE10" s="4">
-        <v>0</v>
-      </c>
-      <c r="AF10" s="4">
-        <v>0</v>
-      </c>
-      <c r="AG10" s="4">
-        <v>0</v>
-      </c>
-      <c r="AH10" s="4">
-        <v>0</v>
-      </c>
-      <c r="AI10" s="4">
-        <v>0</v>
-      </c>
-      <c r="AJ10" s="4">
-        <v>0</v>
-      </c>
-      <c r="AK10" s="4">
-        <v>0</v>
-      </c>
-      <c r="AL10" s="4">
-        <v>0</v>
-      </c>
-      <c r="AM10" s="4">
-        <v>0</v>
-      </c>
-      <c r="AN10" s="4">
-        <v>0</v>
-      </c>
-      <c r="AO10" s="4">
-        <v>0</v>
-      </c>
-      <c r="AP10" s="4">
-        <v>0</v>
-      </c>
-      <c r="AQ10" s="4">
-        <v>0</v>
-      </c>
-      <c r="AR10" s="4">
-        <v>0</v>
-      </c>
-      <c r="AS10" s="4">
-        <v>0</v>
-      </c>
-      <c r="AT10" s="4">
-        <v>0</v>
-      </c>
-      <c r="AU10" s="4">
-        <v>0</v>
-      </c>
-      <c r="AV10" s="4">
-        <v>0</v>
-      </c>
-      <c r="AW10" s="4">
-        <v>0</v>
-      </c>
-      <c r="AX10" s="4">
-        <v>0</v>
-      </c>
-      <c r="AY10" s="4">
-        <v>0</v>
-      </c>
-      <c r="AZ10" s="4">
-        <v>0</v>
-      </c>
-      <c r="BA10" s="4">
-        <v>0</v>
-      </c>
-      <c r="BB10" s="4">
-        <v>0</v>
-      </c>
-      <c r="BC10" s="4">
-        <v>0</v>
-      </c>
-      <c r="BD10" s="4">
-        <v>0</v>
-      </c>
-      <c r="BE10" s="4">
-        <v>0</v>
-      </c>
-      <c r="BF10" s="4">
-        <v>0</v>
-      </c>
-      <c r="BG10" s="4">
-        <v>0</v>
-      </c>
-      <c r="BH10" s="4">
-        <v>0</v>
-      </c>
-      <c r="BI10" s="4">
-        <v>0</v>
-      </c>
-      <c r="BJ10" s="4">
-        <v>0</v>
-      </c>
-      <c r="BK10" s="4">
-        <v>0</v>
-      </c>
-      <c r="BL10" s="4">
-        <v>0</v>
-      </c>
-      <c r="BM10" s="4">
-        <v>0</v>
-      </c>
-      <c r="BN10" s="4">
-        <v>0</v>
-      </c>
-      <c r="BO10" s="4">
-        <v>0</v>
-      </c>
-      <c r="BP10" s="4">
-        <v>0</v>
-      </c>
-      <c r="BQ10" s="4">
-        <v>0</v>
-      </c>
-      <c r="BR10" s="4">
-        <v>0</v>
-      </c>
-      <c r="BS10" s="4">
-        <v>0</v>
-      </c>
-      <c r="BT10" s="4">
-        <v>0</v>
-      </c>
-      <c r="BU10" s="4">
-        <v>0</v>
-      </c>
-      <c r="BV10" s="4">
-        <v>0</v>
-      </c>
-      <c r="BW10" s="4">
-        <v>0</v>
-      </c>
-      <c r="BX10" s="4">
-        <v>0</v>
-      </c>
-      <c r="BY10" s="4">
-        <v>0</v>
-      </c>
-      <c r="BZ10" s="4">
-        <v>0</v>
-      </c>
-      <c r="CA10" s="4">
-        <v>0</v>
-      </c>
-      <c r="CB10" s="4">
-        <v>0</v>
-      </c>
-      <c r="CC10" s="4">
-        <v>0</v>
-      </c>
-      <c r="CD10" s="4">
-        <v>0</v>
-      </c>
-      <c r="CE10" s="4">
-        <v>0</v>
-      </c>
-      <c r="CF10" s="4">
-        <v>0</v>
-      </c>
-      <c r="CG10" s="4">
-        <v>0</v>
-      </c>
-      <c r="CH10" s="4">
-        <v>0</v>
-      </c>
-      <c r="CI10" s="4">
-        <v>0</v>
-      </c>
-      <c r="CJ10" s="4">
-        <v>0</v>
-      </c>
-      <c r="CK10" s="4">
-        <v>0</v>
-      </c>
-      <c r="CL10" s="4">
-        <v>0</v>
-      </c>
-      <c r="CM10" s="4">
-        <v>0</v>
-      </c>
-      <c r="CN10" s="4">
-        <v>0</v>
-      </c>
-      <c r="CO10" s="4">
-        <v>0</v>
-      </c>
-      <c r="CP10" s="4">
-        <v>0</v>
-      </c>
-      <c r="CQ10" s="4">
-        <v>0</v>
-      </c>
-      <c r="CR10" s="4">
-        <v>0</v>
-      </c>
-      <c r="CS10" s="4">
-        <v>0</v>
-      </c>
-      <c r="CT10" s="4">
-        <v>0</v>
-      </c>
-      <c r="CU10" s="4">
-        <v>0</v>
-      </c>
-      <c r="CV10" s="4">
-        <v>0</v>
-      </c>
-      <c r="CW10" s="4">
-        <v>0</v>
-      </c>
-      <c r="CX10" s="4">
-        <v>0</v>
-      </c>
-      <c r="CY10" s="4">
-        <v>0</v>
-      </c>
-      <c r="CZ10" s="4">
-        <v>0</v>
-      </c>
-      <c r="DA10" s="4">
-        <v>0</v>
-      </c>
-      <c r="DB10" s="4">
-        <v>0</v>
-      </c>
-      <c r="DC10" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="2:107" x14ac:dyDescent="0.25">
-      <c r="B11" s="3" t="s">
-        <v>200</v>
-      </c>
-      <c r="C11" s="4">
-        <v>1</v>
-      </c>
-      <c r="D11" s="4">
-        <v>1</v>
-      </c>
-      <c r="E11" s="4">
-        <v>1</v>
-      </c>
-      <c r="F11" s="4">
-        <v>1</v>
-      </c>
-      <c r="G11" s="4">
-        <v>1</v>
-      </c>
-      <c r="H11" s="4">
-        <v>1</v>
-      </c>
-      <c r="I11" s="4">
-        <v>1</v>
-      </c>
-      <c r="J11" s="4">
-        <v>2</v>
-      </c>
-      <c r="K11" s="4">
-        <v>2</v>
-      </c>
-      <c r="L11" s="4">
-        <v>2</v>
-      </c>
-      <c r="M11" s="4">
-        <v>2</v>
-      </c>
-      <c r="N11" s="4">
-        <v>2</v>
-      </c>
-      <c r="O11" s="4">
-        <v>1</v>
-      </c>
-      <c r="P11" s="4">
-        <v>1</v>
-      </c>
-      <c r="Q11" s="4">
-        <v>1</v>
-      </c>
-      <c r="R11" s="4">
-        <v>1</v>
-      </c>
-      <c r="S11" s="4">
-        <v>1</v>
-      </c>
-      <c r="T11" s="4">
-        <v>1</v>
-      </c>
-      <c r="U11" s="4">
-        <v>2</v>
-      </c>
-      <c r="V11" s="4">
-        <v>2</v>
-      </c>
-      <c r="W11" s="4">
-        <v>2</v>
-      </c>
-      <c r="X11" s="4">
-        <v>2</v>
-      </c>
-      <c r="Y11" s="4">
-        <v>2</v>
-      </c>
-      <c r="Z11" s="4">
-        <v>2</v>
-      </c>
-      <c r="AA11" s="4">
-        <v>2</v>
-      </c>
-      <c r="AB11" s="4">
-        <v>2</v>
-      </c>
-      <c r="AC11" s="4">
-        <v>2</v>
-      </c>
-      <c r="AD11" s="4">
-        <v>1</v>
-      </c>
-      <c r="AE11" s="4">
-        <v>1</v>
-      </c>
-      <c r="AF11" s="4">
-        <v>2</v>
-      </c>
-      <c r="AG11" s="4">
-        <v>2</v>
-      </c>
-      <c r="AH11" s="4">
-        <v>2</v>
-      </c>
-      <c r="AI11" s="4">
-        <v>2</v>
-      </c>
-      <c r="AJ11" s="4">
-        <v>2</v>
-      </c>
-      <c r="AK11" s="4">
-        <v>2</v>
-      </c>
-      <c r="AL11" s="4">
-        <v>2</v>
-      </c>
-      <c r="AM11" s="4">
-        <v>2</v>
-      </c>
-      <c r="AN11" s="4">
-        <v>2</v>
-      </c>
-      <c r="AO11" s="4">
-        <v>2</v>
-      </c>
-      <c r="AP11" s="4">
-        <v>2</v>
-      </c>
-      <c r="AQ11" s="4">
-        <v>2</v>
-      </c>
-      <c r="AR11" s="4">
-        <v>1</v>
-      </c>
-      <c r="AS11" s="4">
-        <v>1</v>
-      </c>
-      <c r="AT11" s="4">
-        <v>1</v>
-      </c>
-      <c r="AU11" s="4">
-        <v>1</v>
-      </c>
-      <c r="AV11" s="4">
-        <v>1</v>
-      </c>
-      <c r="AW11" s="4">
-        <v>1</v>
-      </c>
-      <c r="AX11" s="4">
-        <v>2</v>
-      </c>
-      <c r="AY11" s="4">
-        <v>1</v>
-      </c>
-      <c r="AZ11" s="4">
-        <v>2</v>
-      </c>
-      <c r="BA11" s="4">
-        <v>2</v>
-      </c>
-      <c r="BB11" s="4">
-        <v>2</v>
-      </c>
-      <c r="BC11" s="4">
-        <v>1</v>
-      </c>
-      <c r="BD11" s="4">
-        <v>1</v>
-      </c>
-      <c r="BE11" s="4">
-        <v>1</v>
-      </c>
-      <c r="BF11" s="4">
-        <v>1</v>
-      </c>
-      <c r="BG11" s="4">
-        <v>2</v>
-      </c>
-      <c r="BH11" s="4">
-        <v>2</v>
-      </c>
-      <c r="BI11" s="4">
-        <v>2</v>
-      </c>
-      <c r="BJ11" s="4">
-        <v>2</v>
-      </c>
-      <c r="BK11" s="4">
-        <v>1</v>
-      </c>
-      <c r="BL11" s="4">
-        <v>1</v>
-      </c>
-      <c r="BM11" s="4">
-        <v>1</v>
-      </c>
-      <c r="BN11" s="4">
-        <v>2</v>
-      </c>
-      <c r="BO11" s="4">
-        <v>1</v>
-      </c>
-      <c r="BP11" s="4">
-        <v>1</v>
-      </c>
-      <c r="BQ11" s="4">
-        <v>1</v>
-      </c>
-      <c r="BR11" s="4">
-        <v>1</v>
-      </c>
-      <c r="BS11" s="4">
-        <v>1</v>
-      </c>
-      <c r="BT11" s="4">
-        <v>2</v>
-      </c>
-      <c r="BU11" s="4">
-        <v>2</v>
-      </c>
-      <c r="BV11" s="4">
-        <v>2</v>
-      </c>
-      <c r="BW11" s="4">
-        <v>2</v>
-      </c>
-      <c r="BX11" s="4">
-        <v>2</v>
-      </c>
-      <c r="BY11" s="4">
-        <v>2</v>
-      </c>
-      <c r="BZ11" s="4">
-        <v>2</v>
-      </c>
-      <c r="CA11" s="4">
-        <v>2</v>
-      </c>
-      <c r="CB11" s="4">
-        <v>2</v>
-      </c>
-      <c r="CC11" s="4">
-        <v>2</v>
-      </c>
-      <c r="CD11" s="4">
-        <v>2</v>
-      </c>
-      <c r="CE11" s="4">
-        <v>2</v>
-      </c>
-      <c r="CF11" s="4">
-        <v>2</v>
-      </c>
-      <c r="CG11" s="4">
-        <v>1</v>
-      </c>
-      <c r="CH11" s="4">
-        <v>1</v>
-      </c>
-      <c r="CI11" s="4">
-        <v>1</v>
-      </c>
-      <c r="CJ11" s="4">
-        <v>1</v>
-      </c>
-      <c r="CK11" s="4">
-        <v>1</v>
-      </c>
-      <c r="CL11" s="4">
-        <v>1</v>
-      </c>
-      <c r="CM11" s="4">
-        <v>1</v>
-      </c>
-      <c r="CN11" s="4">
-        <v>1</v>
-      </c>
-      <c r="CO11" s="4">
-        <v>2</v>
-      </c>
-      <c r="CP11" s="4">
-        <v>2</v>
-      </c>
-      <c r="CQ11" s="4">
-        <v>2</v>
-      </c>
-      <c r="CR11" s="4">
-        <v>1</v>
-      </c>
-      <c r="CS11" s="4">
-        <v>1</v>
-      </c>
-      <c r="CT11" s="4">
-        <v>1</v>
-      </c>
-      <c r="CU11" s="4">
-        <v>2</v>
-      </c>
-      <c r="CV11" s="4">
-        <v>1</v>
-      </c>
-      <c r="CW11" s="4">
-        <v>2</v>
-      </c>
-      <c r="CX11" s="4">
-        <v>1</v>
-      </c>
-      <c r="CY11" s="4">
-        <v>2</v>
-      </c>
-      <c r="CZ11" s="4">
-        <v>1</v>
-      </c>
-      <c r="DA11" s="4">
-        <v>2</v>
-      </c>
-      <c r="DB11" s="4">
-        <v>2</v>
-      </c>
-      <c r="DC11" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="2:107" x14ac:dyDescent="0.25">
-      <c r="B12" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="C12" s="4">
-        <v>1</v>
-      </c>
-      <c r="D12" s="4">
-        <v>1</v>
-      </c>
-      <c r="E12" s="4">
-        <v>1</v>
-      </c>
-      <c r="F12" s="4">
-        <v>1</v>
-      </c>
-      <c r="G12" s="4">
-        <v>1</v>
-      </c>
-      <c r="H12" s="4">
-        <v>1</v>
-      </c>
-      <c r="I12" s="4">
-        <v>1</v>
-      </c>
-      <c r="J12" s="4">
-        <v>0</v>
-      </c>
-      <c r="K12" s="4">
-        <v>1</v>
-      </c>
-      <c r="L12" s="4">
-        <v>1</v>
-      </c>
-      <c r="M12" s="4">
-        <v>1</v>
-      </c>
-      <c r="N12" s="4">
-        <v>1</v>
-      </c>
-      <c r="O12" s="9"/>
-      <c r="P12" s="9"/>
-      <c r="Q12" s="9"/>
-      <c r="R12" s="9"/>
-      <c r="S12" s="9"/>
-      <c r="T12" s="9"/>
-      <c r="U12" s="9"/>
-      <c r="V12" s="9"/>
-      <c r="W12" s="9"/>
-      <c r="X12" s="9"/>
-      <c r="Y12" s="9"/>
-      <c r="Z12" s="9"/>
-      <c r="AA12" s="4">
-        <v>1</v>
-      </c>
-      <c r="AB12" s="4">
-        <v>0</v>
-      </c>
-      <c r="AC12" s="4">
-        <v>0</v>
-      </c>
-      <c r="AD12" s="4">
-        <v>0</v>
-      </c>
-      <c r="AE12" s="4">
-        <v>0</v>
-      </c>
-      <c r="AF12" s="4">
-        <v>0</v>
-      </c>
-      <c r="AG12" s="4">
-        <v>0</v>
-      </c>
-      <c r="AH12" s="4">
-        <v>0</v>
-      </c>
-      <c r="AI12" s="4">
-        <v>0</v>
-      </c>
-      <c r="AJ12" s="4">
-        <v>0</v>
-      </c>
-      <c r="AK12" s="4">
-        <v>0</v>
-      </c>
-      <c r="AL12" s="4">
-        <v>0</v>
-      </c>
-      <c r="AM12" s="4">
-        <v>0</v>
-      </c>
-      <c r="AN12" s="4">
-        <v>0</v>
-      </c>
-      <c r="AO12" s="4">
-        <v>0</v>
-      </c>
-      <c r="AP12" s="4">
-        <v>0</v>
-      </c>
-      <c r="AQ12" s="4">
-        <v>0</v>
-      </c>
-      <c r="AR12" s="4">
-        <v>0</v>
-      </c>
-      <c r="AS12" s="4">
-        <v>0</v>
-      </c>
-      <c r="AT12" s="4">
-        <v>0</v>
-      </c>
-      <c r="AU12" s="4">
-        <v>0</v>
-      </c>
-      <c r="AV12" s="4">
-        <v>0</v>
-      </c>
-      <c r="AW12" s="4">
-        <v>0</v>
-      </c>
-      <c r="AX12" s="4">
-        <v>0</v>
-      </c>
-      <c r="AY12" s="4">
-        <v>0</v>
-      </c>
-      <c r="AZ12" s="4">
-        <v>0</v>
-      </c>
-      <c r="BA12" s="4">
-        <v>0</v>
-      </c>
-      <c r="BB12" s="4">
-        <v>0</v>
-      </c>
-      <c r="BC12" s="4">
-        <v>0</v>
-      </c>
-      <c r="BD12" s="4">
-        <v>0</v>
-      </c>
-      <c r="BE12" s="4">
-        <v>0</v>
-      </c>
-      <c r="BF12" s="4">
-        <v>0</v>
-      </c>
-      <c r="BG12" s="4">
-        <v>0</v>
-      </c>
-      <c r="BH12" s="4">
-        <v>0</v>
-      </c>
-      <c r="BI12" s="4">
-        <v>0</v>
-      </c>
-      <c r="BJ12" s="4">
-        <v>0</v>
-      </c>
-      <c r="BK12" s="4">
-        <v>0</v>
-      </c>
-      <c r="BL12" s="4">
-        <v>0</v>
-      </c>
-      <c r="BM12" s="4">
-        <v>0</v>
-      </c>
-      <c r="BN12" s="4">
-        <v>0</v>
-      </c>
-      <c r="BO12" s="4">
-        <v>0</v>
-      </c>
-      <c r="BP12" s="4">
-        <v>0</v>
-      </c>
-      <c r="BQ12" s="4">
-        <v>0</v>
-      </c>
-      <c r="BR12" s="4">
-        <v>0</v>
-      </c>
-      <c r="BS12" s="4">
-        <v>0</v>
-      </c>
-      <c r="BT12" s="4">
-        <v>0</v>
-      </c>
-      <c r="BU12" s="4">
-        <v>0</v>
-      </c>
-      <c r="BV12" s="4">
-        <v>0</v>
-      </c>
-      <c r="BW12" s="4">
-        <v>0</v>
-      </c>
-      <c r="BX12" s="4">
-        <v>0</v>
-      </c>
-      <c r="BY12" s="4">
-        <v>0</v>
-      </c>
-      <c r="BZ12" s="4">
-        <v>0</v>
-      </c>
-      <c r="CA12" s="4">
-        <v>0</v>
-      </c>
-      <c r="CB12" s="4">
-        <v>0</v>
-      </c>
-      <c r="CC12" s="4">
-        <v>0</v>
-      </c>
-      <c r="CD12" s="4">
-        <v>0</v>
-      </c>
-      <c r="CE12" s="4">
-        <v>0</v>
-      </c>
-      <c r="CF12" s="4">
-        <v>0</v>
-      </c>
-      <c r="CG12" s="4">
-        <v>0</v>
-      </c>
-      <c r="CH12" s="4">
-        <v>0</v>
-      </c>
-      <c r="CI12" s="4">
-        <v>0</v>
-      </c>
-      <c r="CJ12" s="4">
-        <v>0</v>
-      </c>
-      <c r="CK12" s="4">
-        <v>0</v>
-      </c>
-      <c r="CL12" s="4">
-        <v>0</v>
-      </c>
-      <c r="CM12" s="4">
-        <v>0</v>
-      </c>
-      <c r="CN12" s="4">
-        <v>0</v>
-      </c>
-      <c r="CO12" s="4">
-        <v>0</v>
-      </c>
-      <c r="CP12" s="4">
-        <v>0</v>
-      </c>
-      <c r="CQ12" s="4">
-        <v>0</v>
-      </c>
-      <c r="CR12" s="4">
-        <v>0</v>
-      </c>
-      <c r="CS12" s="4">
-        <v>0</v>
-      </c>
-      <c r="CT12" s="4">
-        <v>0</v>
-      </c>
-      <c r="CU12" s="4">
-        <v>0</v>
-      </c>
-      <c r="CV12" s="4">
-        <v>0</v>
-      </c>
-      <c r="CW12" s="4">
-        <v>0</v>
-      </c>
-      <c r="CX12" s="4">
-        <v>0</v>
-      </c>
-      <c r="CY12" s="4">
-        <v>0</v>
-      </c>
-      <c r="CZ12" s="4">
-        <v>0</v>
-      </c>
-      <c r="DA12" s="4">
-        <v>0</v>
-      </c>
-      <c r="DB12" s="4">
-        <v>0</v>
-      </c>
-      <c r="DC12" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="2:107" x14ac:dyDescent="0.25">
-      <c r="B13" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="C13" s="4"/>
-      <c r="D13" s="4">
-        <v>1</v>
-      </c>
-      <c r="E13" s="4">
-        <v>1</v>
-      </c>
-      <c r="F13" s="4">
-        <v>1</v>
-      </c>
-      <c r="G13" s="4">
-        <v>2</v>
-      </c>
-      <c r="H13" s="4">
-        <v>2</v>
-      </c>
-      <c r="I13" s="4">
-        <v>2</v>
-      </c>
-      <c r="J13" s="4"/>
-      <c r="K13" s="4"/>
-      <c r="L13" s="5">
+        <v>2</v>
+      </c>
+      <c r="J10" s="4"/>
+      <c r="K10" s="4"/>
+      <c r="L10" s="5">
         <v>3</v>
       </c>
-      <c r="M13" s="5">
+      <c r="M10" s="5">
         <v>3</v>
       </c>
-      <c r="N13" s="4"/>
-      <c r="O13" s="4"/>
-      <c r="P13" s="4"/>
-      <c r="Q13" s="4"/>
-      <c r="R13" s="4"/>
-      <c r="S13" s="4"/>
-      <c r="T13" s="4"/>
-      <c r="U13" s="4"/>
-      <c r="V13" s="4"/>
-      <c r="W13" s="4"/>
-      <c r="X13" s="4"/>
-      <c r="Y13" s="4"/>
-      <c r="Z13" s="4"/>
-      <c r="AA13" s="4"/>
-      <c r="AB13" s="4"/>
-      <c r="AC13" s="4"/>
-      <c r="AD13" s="4"/>
-      <c r="AE13" s="4"/>
-      <c r="AF13" s="4"/>
-      <c r="AG13" s="4"/>
-      <c r="AH13" s="4"/>
-      <c r="AI13" s="4"/>
-      <c r="AJ13" s="4"/>
-      <c r="AK13" s="4"/>
-      <c r="AL13" s="4"/>
-      <c r="AM13" s="4"/>
-      <c r="AN13" s="4"/>
-      <c r="AO13" s="4"/>
-      <c r="AP13" s="4"/>
-      <c r="AQ13" s="4"/>
-      <c r="AR13" s="4"/>
-      <c r="AS13" s="4"/>
-      <c r="AT13" s="4"/>
-      <c r="AU13" s="4"/>
-      <c r="AV13" s="4"/>
-      <c r="AW13" s="4"/>
-      <c r="AX13" s="4"/>
-      <c r="AY13" s="4"/>
-      <c r="AZ13" s="4"/>
-      <c r="BA13" s="4"/>
-      <c r="BB13" s="4"/>
-      <c r="BC13" s="4"/>
-      <c r="BD13" s="4"/>
-      <c r="BE13" s="4"/>
-      <c r="BF13" s="4"/>
-      <c r="BG13" s="4"/>
-      <c r="BH13" s="4"/>
-      <c r="BI13" s="4"/>
-      <c r="BJ13" s="4"/>
-      <c r="BK13" s="4"/>
-      <c r="BL13" s="4"/>
-      <c r="BM13" s="4"/>
-      <c r="BN13" s="4"/>
-      <c r="BO13" s="4"/>
-      <c r="BP13" s="4"/>
-      <c r="BQ13" s="4"/>
-      <c r="BR13" s="4"/>
-      <c r="BS13" s="4"/>
-      <c r="BT13" s="4"/>
-      <c r="BU13" s="4"/>
-      <c r="BV13" s="4"/>
-      <c r="BW13" s="4"/>
-      <c r="BX13" s="4"/>
-      <c r="BY13" s="4"/>
-      <c r="BZ13" s="4"/>
-      <c r="CA13" s="4"/>
-      <c r="CB13" s="4"/>
-      <c r="CC13" s="4"/>
-      <c r="CD13" s="4"/>
-      <c r="CE13" s="4"/>
-      <c r="CF13" s="4"/>
-      <c r="CG13" s="4"/>
-      <c r="CH13" s="4"/>
-      <c r="CI13" s="4"/>
-      <c r="CJ13" s="4"/>
-      <c r="CK13" s="4"/>
-      <c r="CL13" s="4"/>
-      <c r="CM13" s="4"/>
-      <c r="CN13" s="4"/>
-      <c r="CO13" s="4"/>
-      <c r="CP13" s="4"/>
-      <c r="CQ13" s="4"/>
-      <c r="CR13" s="4"/>
-      <c r="CS13" s="4"/>
-      <c r="CT13" s="4"/>
-      <c r="CU13" s="4"/>
-      <c r="CV13" s="4"/>
-      <c r="CW13" s="4"/>
-      <c r="CX13" s="4"/>
-      <c r="CY13" s="4"/>
-      <c r="CZ13" s="4"/>
-      <c r="DA13" s="4"/>
-      <c r="DB13" s="4"/>
-      <c r="DC13" s="4"/>
-    </row>
-    <row r="14" spans="2:107" x14ac:dyDescent="0.25">
-      <c r="B14" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="AB14" s="7"/>
-      <c r="AC14" s="7"/>
-    </row>
-    <row r="15" spans="2:107" x14ac:dyDescent="0.25">
-      <c r="B15" s="6" t="s">
-        <v>191</v>
-      </c>
-      <c r="O15">
-        <v>1</v>
-      </c>
-      <c r="P15">
-        <v>1</v>
-      </c>
-      <c r="Q15">
-        <v>1</v>
-      </c>
-      <c r="R15">
-        <v>1</v>
-      </c>
-      <c r="S15">
-        <v>1</v>
-      </c>
-      <c r="T15">
-        <v>1</v>
-      </c>
-      <c r="U15">
-        <v>1</v>
-      </c>
-      <c r="V15">
-        <v>1</v>
-      </c>
-      <c r="W15">
-        <v>1</v>
-      </c>
-      <c r="X15">
-        <v>1</v>
-      </c>
-      <c r="Y15">
-        <v>1</v>
-      </c>
-      <c r="Z15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B19" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="24" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B24" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="25" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B25" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="26" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B26" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="27" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B27" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="28" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B28" t="s">
-        <v>148</v>
-      </c>
+      <c r="N10" s="4"/>
+      <c r="O10" s="4"/>
+      <c r="P10" s="4"/>
+      <c r="Q10" s="4"/>
+      <c r="R10" s="4"/>
+      <c r="S10" s="4"/>
+      <c r="T10" s="4"/>
+      <c r="U10" s="4"/>
+      <c r="V10" s="4"/>
+      <c r="W10" s="4"/>
+      <c r="X10" s="4"/>
+      <c r="Y10" s="4"/>
+      <c r="Z10" s="4"/>
+      <c r="AA10" s="4"/>
+      <c r="AB10" s="4"/>
+      <c r="AC10" s="4"/>
+      <c r="AD10" s="4"/>
+      <c r="AE10" s="4"/>
+      <c r="AF10" s="4"/>
+      <c r="AG10" s="4"/>
+      <c r="AH10" s="4"/>
+      <c r="AI10" s="4"/>
+      <c r="AJ10" s="4"/>
+      <c r="AK10" s="4"/>
+      <c r="AL10" s="4"/>
+      <c r="AM10" s="4"/>
+      <c r="AN10" s="4"/>
+      <c r="AO10" s="4"/>
+      <c r="AP10" s="4"/>
+      <c r="AQ10" s="4"/>
+      <c r="AR10" s="4"/>
+      <c r="AS10" s="4"/>
+      <c r="AT10" s="4"/>
+      <c r="AU10" s="4"/>
+      <c r="AV10" s="4"/>
+      <c r="AW10" s="4"/>
+      <c r="AX10" s="4"/>
+      <c r="AY10" s="4"/>
+      <c r="AZ10" s="4"/>
+      <c r="BA10" s="4"/>
+      <c r="BB10" s="4"/>
+      <c r="BC10" s="4"/>
+      <c r="BD10" s="4"/>
+      <c r="BE10" s="4"/>
+      <c r="BF10" s="4"/>
+      <c r="BG10" s="4"/>
+      <c r="BH10" s="4"/>
+      <c r="BI10" s="4"/>
+      <c r="BJ10" s="4"/>
+      <c r="BK10" s="4"/>
+      <c r="BL10" s="4"/>
+      <c r="BM10" s="4"/>
+      <c r="BN10" s="4"/>
+      <c r="BO10" s="4"/>
+      <c r="BP10" s="4"/>
+      <c r="BQ10" s="4"/>
+      <c r="BR10" s="4"/>
+      <c r="BS10" s="4"/>
+      <c r="BT10" s="4"/>
+      <c r="BU10" s="4"/>
+      <c r="BV10" s="4"/>
+      <c r="BW10" s="4"/>
+      <c r="BX10" s="4"/>
+      <c r="BY10" s="4"/>
+      <c r="BZ10" s="4"/>
+      <c r="CA10" s="4"/>
+      <c r="CB10" s="4"/>
+      <c r="CC10" s="4"/>
+      <c r="CD10" s="4"/>
+      <c r="CE10" s="4"/>
+      <c r="CF10" s="4"/>
+      <c r="CG10" s="4"/>
+      <c r="CH10" s="4"/>
+      <c r="CI10" s="4"/>
+      <c r="CJ10" s="4"/>
+      <c r="CK10" s="4"/>
+      <c r="CL10" s="4"/>
+      <c r="CM10" s="4"/>
+      <c r="CN10" s="4"/>
+      <c r="CO10" s="4"/>
+      <c r="CP10" s="4"/>
+      <c r="CQ10" s="4"/>
+      <c r="CR10" s="4"/>
+      <c r="CS10" s="4"/>
+      <c r="CT10" s="4"/>
+      <c r="CU10" s="4"/>
+      <c r="CV10" s="4"/>
+      <c r="CW10" s="4"/>
+      <c r="CX10" s="4"/>
+      <c r="CY10" s="4"/>
+      <c r="CZ10" s="4"/>
+      <c r="DA10" s="4"/>
+      <c r="DB10" s="4"/>
+      <c r="DC10" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -4153,7 +3245,7 @@
         <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>197</v>
+        <v>186</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -4161,7 +3253,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>198</v>
+        <v>187</v>
       </c>
     </row>
   </sheetData>
@@ -4173,7 +3265,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F75"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
@@ -4204,7 +3296,7 @@
         <v>3</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -4221,10 +3313,10 @@
         <v>7</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -4241,10 +3333,10 @@
         <v>7</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -4261,10 +3353,10 @@
         <v>7</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -4281,10 +3373,10 @@
         <v>7</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -4301,10 +3393,10 @@
         <v>7</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -4321,10 +3413,10 @@
         <v>7</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -4341,10 +3433,10 @@
         <v>7</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -4361,10 +3453,10 @@
         <v>8</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -4381,10 +3473,10 @@
         <v>8</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -4401,10 +3493,10 @@
         <v>8</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -4421,10 +3513,10 @@
         <v>8</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -4435,16 +3527,16 @@
         <v>4</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>209</v>
+        <v>198</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -4459,7 +3551,7 @@
         <v>7</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F14" s="1" t="s">
         <v>16</v>
@@ -4509,7 +3601,7 @@
         <v>7</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F17" s="1" t="s">
         <v>18</v>
@@ -4559,7 +3651,7 @@
         <v>8</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F20" s="1" t="s">
         <v>21</v>
@@ -4609,7 +3701,7 @@
         <v>8</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F23" s="1" t="s">
         <v>24</v>
@@ -4655,16 +3747,16 @@
         <v>4</v>
       </c>
       <c r="C26" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="D26" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>192</v>
+        <v>181</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
@@ -4672,19 +3764,19 @@
         <v>26</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="D27" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
@@ -4692,19 +3784,19 @@
         <v>27</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="D28" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
@@ -4712,19 +3804,19 @@
         <v>28</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>194</v>
+        <v>183</v>
       </c>
       <c r="D29" s="1" t="s">
         <v>7</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>193</v>
+        <v>182</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
@@ -4732,19 +3824,19 @@
         <v>29</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>195</v>
+        <v>184</v>
       </c>
       <c r="D30" s="1" t="s">
         <v>7</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>196</v>
+        <v>185</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
@@ -4752,19 +3844,19 @@
         <v>30</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="D31" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
@@ -4772,19 +3864,19 @@
         <v>31</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="D32" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
@@ -4792,19 +3884,19 @@
         <v>32</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="D33" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
@@ -4812,19 +3904,19 @@
         <v>33</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="D34" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E34" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="F34" s="1" t="s">
         <v>82</v>
-      </c>
-      <c r="F34" s="1" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
@@ -4832,19 +3924,19 @@
         <v>34</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="D35" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
@@ -4852,19 +3944,19 @@
         <v>35</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="D36" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
@@ -4872,19 +3964,19 @@
         <v>36</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="D37" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
@@ -4892,19 +3984,19 @@
         <v>37</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="D38" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
@@ -4912,19 +4004,19 @@
         <v>38</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="D39" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
@@ -4932,19 +4024,19 @@
         <v>39</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="D40" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
@@ -4952,19 +4044,19 @@
         <v>40</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="D41" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
@@ -4972,19 +4064,19 @@
         <v>41</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="D42" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
@@ -4992,19 +4084,19 @@
         <v>42</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="D43" s="1" t="s">
         <v>7</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
@@ -5012,19 +4104,19 @@
         <v>43</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="D44" s="1" t="s">
         <v>7</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
@@ -5032,19 +4124,19 @@
         <v>44</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
       <c r="D45" s="1" t="s">
         <v>7</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
@@ -5052,19 +4144,19 @@
         <v>45</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
       <c r="D46" s="1" t="s">
         <v>7</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
@@ -5072,19 +4164,19 @@
         <v>46</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="D47" s="1" t="s">
         <v>7</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
@@ -5092,19 +4184,19 @@
         <v>47</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
       <c r="D48" s="1" t="s">
         <v>7</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
@@ -5112,19 +4204,19 @@
         <v>48</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
       <c r="D49" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
@@ -5132,19 +4224,19 @@
         <v>49</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
       <c r="D50" s="1" t="s">
         <v>7</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>131</v>
+        <v>122</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>132</v>
+        <v>123</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
@@ -5152,19 +4244,19 @@
         <v>50</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>135</v>
+        <v>126</v>
       </c>
       <c r="D51" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>134</v>
+        <v>125</v>
       </c>
       <c r="F51" t="s">
-        <v>136</v>
+        <v>127</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
@@ -5172,19 +4264,19 @@
         <v>51</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>138</v>
+        <v>129</v>
       </c>
       <c r="D52" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>134</v>
+        <v>125</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>139</v>
+        <v>130</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
@@ -5192,19 +4284,19 @@
         <v>52</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>140</v>
+        <v>131</v>
       </c>
       <c r="D53" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>141</v>
+        <v>132</v>
       </c>
       <c r="F53" s="1" t="s">
-        <v>142</v>
+        <v>133</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
@@ -5212,19 +4304,19 @@
         <v>53</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>144</v>
+        <v>135</v>
       </c>
       <c r="D54" s="1" t="s">
         <v>7</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>146</v>
+        <v>137</v>
       </c>
       <c r="F54" s="1" t="s">
-        <v>145</v>
+        <v>136</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
@@ -5232,19 +4324,19 @@
         <v>54</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>150</v>
+        <v>140</v>
       </c>
       <c r="D55" s="1" t="s">
         <v>7</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>149</v>
+        <v>139</v>
       </c>
       <c r="F55" s="1" t="s">
-        <v>153</v>
+        <v>143</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
@@ -5252,19 +4344,19 @@
         <v>55</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>151</v>
+        <v>141</v>
       </c>
       <c r="D56" s="1" t="s">
         <v>7</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>149</v>
+        <v>139</v>
       </c>
       <c r="F56" s="1" t="s">
-        <v>154</v>
+        <v>144</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
@@ -5272,19 +4364,19 @@
         <v>56</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>152</v>
+        <v>142</v>
       </c>
       <c r="D57" s="1" t="s">
         <v>7</v>
       </c>
       <c r="E57" s="1" t="s">
-        <v>149</v>
+        <v>139</v>
       </c>
       <c r="F57" s="1" t="s">
-        <v>155</v>
+        <v>145</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
@@ -5292,19 +4384,19 @@
         <v>57</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>157</v>
+        <v>147</v>
       </c>
       <c r="D58" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>156</v>
+        <v>146</v>
       </c>
       <c r="F58" s="1" t="s">
-        <v>159</v>
+        <v>149</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
@@ -5312,19 +4404,19 @@
         <v>58</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>158</v>
+        <v>148</v>
       </c>
       <c r="D59" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>156</v>
+        <v>146</v>
       </c>
       <c r="F59" s="1" t="s">
-        <v>160</v>
+        <v>150</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
@@ -5332,19 +4424,19 @@
         <v>59</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>162</v>
+        <v>152</v>
       </c>
       <c r="D60" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>161</v>
+        <v>151</v>
       </c>
       <c r="F60" s="1" t="s">
-        <v>165</v>
+        <v>155</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
@@ -5352,19 +4444,19 @@
         <v>60</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="C61" t="s">
-        <v>163</v>
+        <v>153</v>
       </c>
       <c r="D61" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>161</v>
+        <v>151</v>
       </c>
       <c r="F61" s="1" t="s">
-        <v>164</v>
+        <v>154</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
@@ -5372,19 +4464,19 @@
         <v>61</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="C62" t="s">
-        <v>169</v>
+        <v>159</v>
       </c>
       <c r="D62" s="1" t="s">
         <v>7</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>168</v>
+        <v>158</v>
       </c>
       <c r="F62" s="1" t="s">
-        <v>170</v>
+        <v>160</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
@@ -5392,19 +4484,19 @@
         <v>62</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="C63" t="s">
-        <v>171</v>
+        <v>161</v>
       </c>
       <c r="D63" s="1" t="s">
         <v>7</v>
       </c>
       <c r="E63" s="1" t="s">
-        <v>168</v>
+        <v>158</v>
       </c>
       <c r="F63" s="1" t="s">
-        <v>172</v>
+        <v>162</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
@@ -5412,19 +4504,19 @@
         <v>63</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="C64" t="s">
-        <v>173</v>
+        <v>163</v>
       </c>
       <c r="D64" s="1" t="s">
         <v>7</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>168</v>
+        <v>158</v>
       </c>
       <c r="F64" s="1" t="s">
-        <v>174</v>
+        <v>164</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
@@ -5432,19 +4524,19 @@
         <v>64</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="C65" t="s">
-        <v>175</v>
+        <v>165</v>
       </c>
       <c r="D65" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>176</v>
+        <v>166</v>
       </c>
       <c r="F65" s="1" t="s">
-        <v>177</v>
+        <v>167</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
@@ -5452,16 +4544,16 @@
         <v>65</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>179</v>
+        <v>169</v>
       </c>
       <c r="C66" t="s">
-        <v>180</v>
+        <v>170</v>
       </c>
       <c r="D66" s="1" t="s">
         <v>7</v>
       </c>
       <c r="E66" s="1" t="s">
-        <v>190</v>
+        <v>180</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
@@ -5469,10 +4561,10 @@
         <v>66</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>179</v>
+        <v>169</v>
       </c>
       <c r="C67" t="s">
-        <v>181</v>
+        <v>171</v>
       </c>
       <c r="D67" s="1" t="s">
         <v>7</v>
@@ -5483,10 +4575,10 @@
         <v>67</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>179</v>
+        <v>169</v>
       </c>
       <c r="C68" t="s">
-        <v>182</v>
+        <v>172</v>
       </c>
       <c r="D68" s="1" t="s">
         <v>7</v>
@@ -5497,10 +4589,10 @@
         <v>68</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>179</v>
+        <v>169</v>
       </c>
       <c r="C69" t="s">
-        <v>183</v>
+        <v>173</v>
       </c>
       <c r="D69" s="1" t="s">
         <v>7</v>
@@ -5511,10 +4603,10 @@
         <v>69</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>179</v>
+        <v>169</v>
       </c>
       <c r="C70" t="s">
-        <v>184</v>
+        <v>174</v>
       </c>
       <c r="D70" s="1" t="s">
         <v>7</v>
@@ -5525,10 +4617,10 @@
         <v>70</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>179</v>
+        <v>169</v>
       </c>
       <c r="C71" t="s">
-        <v>185</v>
+        <v>175</v>
       </c>
       <c r="D71" s="1" t="s">
         <v>8</v>
@@ -5539,10 +4631,10 @@
         <v>71</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>179</v>
+        <v>169</v>
       </c>
       <c r="C72" t="s">
-        <v>186</v>
+        <v>176</v>
       </c>
       <c r="D72" s="1" t="s">
         <v>8</v>
@@ -5553,10 +4645,10 @@
         <v>72</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>179</v>
+        <v>169</v>
       </c>
       <c r="C73" t="s">
-        <v>187</v>
+        <v>177</v>
       </c>
       <c r="D73" s="1" t="s">
         <v>8</v>
@@ -5567,10 +4659,10 @@
         <v>73</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>179</v>
+        <v>169</v>
       </c>
       <c r="C74" t="s">
-        <v>188</v>
+        <v>178</v>
       </c>
       <c r="D74" s="1" t="s">
         <v>8</v>
@@ -5581,10 +4673,10 @@
         <v>74</v>
       </c>
       <c r="B75" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="C75" t="s">
         <v>179</v>
-      </c>
-      <c r="C75" t="s">
-        <v>189</v>
       </c>
       <c r="D75" s="1" t="s">
         <v>8</v>
@@ -5611,7 +4703,7 @@
         <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -5619,7 +4711,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -5627,7 +4719,7 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -5635,7 +4727,7 @@
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
     </row>
   </sheetData>
@@ -5657,8 +4749,8 @@
       <c r="A1">
         <v>1</v>
       </c>
-      <c r="B1" s="8" t="s">
-        <v>201</v>
+      <c r="B1" s="6" t="s">
+        <v>190</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -5666,15 +4758,15 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>202</v>
+        <v>191</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>3</v>
       </c>
-      <c r="B3" s="8" t="s">
-        <v>203</v>
+      <c r="B3" s="6" t="s">
+        <v>192</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -5682,50 +4774,50 @@
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>5</v>
       </c>
-      <c r="B5" s="8" t="s">
-        <v>74</v>
+      <c r="B5" s="6" t="s">
+        <v>68</v>
       </c>
       <c r="C5" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>6</v>
       </c>
-      <c r="B6" s="8" t="s">
-        <v>208</v>
+      <c r="B6" s="6" t="s">
+        <v>197</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>7</v>
       </c>
-      <c r="B7" s="8" t="s">
-        <v>207</v>
+      <c r="B7" s="6" t="s">
+        <v>196</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>8</v>
       </c>
-      <c r="B8" s="8" t="s">
-        <v>206</v>
+      <c r="B8" s="6" t="s">
+        <v>195</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>9</v>
       </c>
-      <c r="B9" s="8" t="s">
-        <v>204</v>
+      <c r="B9" s="6" t="s">
+        <v>193</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -5733,7 +4825,7 @@
         <v>10</v>
       </c>
       <c r="B10" t="s">
-        <v>205</v>
+        <v>194</v>
       </c>
     </row>
   </sheetData>
@@ -5756,7 +4848,7 @@
         <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -5764,7 +4856,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -5772,7 +4864,7 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -5780,7 +4872,7 @@
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -5788,7 +4880,7 @@
         <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -5796,7 +4888,7 @@
         <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>133</v>
+        <v>124</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -5804,7 +4896,7 @@
         <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -5812,7 +4904,7 @@
         <v>8</v>
       </c>
       <c r="B8" t="s">
-        <v>143</v>
+        <v>134</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -5820,7 +4912,7 @@
         <v>9</v>
       </c>
       <c r="B9" t="s">
-        <v>147</v>
+        <v>138</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -5828,7 +4920,7 @@
         <v>10</v>
       </c>
       <c r="B10" t="s">
-        <v>166</v>
+        <v>156</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -5836,7 +4928,7 @@
         <v>11</v>
       </c>
       <c r="B11" t="s">
-        <v>167</v>
+        <v>157</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -5844,7 +4936,7 @@
         <v>12</v>
       </c>
       <c r="B12" t="s">
-        <v>178</v>
+        <v>168</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
upd: 0s for single cell in Bulk=1 in design matrix
</commit_message>
<xml_diff>
--- a/DesignMatrix.xlsx
+++ b/DesignMatrix.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11110"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEFF38A3-D00B-4A1E-BF3B-57C38EBE6CF5}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27A1861D-61EB-DF40-AF36-C355F6A38205}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25440" windowHeight="15400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DesignMatrix" sheetId="2" r:id="rId1"/>
@@ -988,18 +988,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F369D9C3-2B00-4B3E-B4DE-89D514952C05}">
   <dimension ref="B2:DC10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AX1" workbookViewId="0">
-      <selection activeCell="CW10" sqref="CW10"/>
+    <sheetView tabSelected="1" topLeftCell="BH1" workbookViewId="0">
+      <selection activeCell="CJ16" sqref="CJ16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="3.85546875" customWidth="1"/>
-    <col min="2" max="2" width="18.85546875" customWidth="1"/>
-    <col min="3" max="107" width="3.85546875" customWidth="1"/>
+    <col min="1" max="1" width="3.83203125" customWidth="1"/>
+    <col min="2" max="2" width="18.83203125" customWidth="1"/>
+    <col min="3" max="107" width="3.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:107" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:107" x14ac:dyDescent="0.2">
       <c r="C2" t="s">
         <v>4</v>
       </c>
@@ -1019,7 +1019,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="3" spans="2:107" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:107" x14ac:dyDescent="0.2">
       <c r="B3" s="3" t="s">
         <v>28</v>
       </c>
@@ -1339,7 +1339,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="4" spans="2:107" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:107" x14ac:dyDescent="0.2">
       <c r="B4" s="3" t="s">
         <v>27</v>
       </c>
@@ -1659,7 +1659,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="2:107" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:107" x14ac:dyDescent="0.2">
       <c r="B5" s="3" t="s">
         <v>29</v>
       </c>
@@ -1979,7 +1979,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="2:107" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:107" x14ac:dyDescent="0.2">
       <c r="B6" s="3" t="s">
         <v>30</v>
       </c>
@@ -2206,100 +2206,100 @@
         <v>1</v>
       </c>
       <c r="BY6" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BZ6" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CA6" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CB6" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CC6" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CD6" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CE6" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CF6" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CG6" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CH6" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CI6" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CJ6" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CK6" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CL6" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CM6" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CN6" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CO6" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CP6" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CQ6" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CR6" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CS6" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CT6" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CU6" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CV6" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CW6" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CX6" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CY6" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CZ6" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="DA6" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="DB6" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="DC6" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="2:107" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="2:107" x14ac:dyDescent="0.2">
       <c r="B7" s="3" t="s">
         <v>39</v>
       </c>
@@ -2459,7 +2459,7 @@
       <c r="DB7" s="4"/>
       <c r="DC7" s="4"/>
     </row>
-    <row r="8" spans="2:107" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:107" x14ac:dyDescent="0.2">
       <c r="B8" s="3" t="s">
         <v>33</v>
       </c>
@@ -2779,7 +2779,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="2:107" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:107" x14ac:dyDescent="0.2">
       <c r="B9" s="3" t="s">
         <v>189</v>
       </c>
@@ -3099,7 +3099,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="2:107" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:107" x14ac:dyDescent="0.2">
       <c r="B10" s="3" t="s">
         <v>57</v>
       </c>
@@ -3238,9 +3238,9 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1">
         <v>1</v>
       </c>
@@ -3248,7 +3248,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>2</v>
       </c>
@@ -3269,17 +3269,17 @@
       <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13.42578125" customWidth="1"/>
-    <col min="2" max="2" width="21.7109375" customWidth="1"/>
-    <col min="3" max="3" width="26.85546875" customWidth="1"/>
-    <col min="4" max="4" width="20.5703125" customWidth="1"/>
-    <col min="5" max="5" width="59.42578125" customWidth="1"/>
+    <col min="1" max="1" width="13.5" customWidth="1"/>
+    <col min="2" max="2" width="21.6640625" customWidth="1"/>
+    <col min="3" max="3" width="26.83203125" customWidth="1"/>
+    <col min="4" max="4" width="20.5" customWidth="1"/>
+    <col min="5" max="5" width="59.5" customWidth="1"/>
     <col min="6" max="6" width="44" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -3299,7 +3299,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -3319,7 +3319,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -3339,7 +3339,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -3359,7 +3359,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -3379,7 +3379,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -3399,7 +3399,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -3419,7 +3419,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -3439,7 +3439,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -3459,7 +3459,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -3479,7 +3479,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -3499,7 +3499,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -3519,7 +3519,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -3539,7 +3539,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -3557,7 +3557,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -3573,7 +3573,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>15</v>
       </c>
@@ -3589,7 +3589,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>16</v>
       </c>
@@ -3607,7 +3607,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>17</v>
       </c>
@@ -3623,7 +3623,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <v>18</v>
       </c>
@@ -3639,7 +3639,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <v>19</v>
       </c>
@@ -3657,7 +3657,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
         <v>20</v>
       </c>
@@ -3673,7 +3673,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
         <v>21</v>
       </c>
@@ -3689,7 +3689,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
         <v>22</v>
       </c>
@@ -3707,7 +3707,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
         <v>23</v>
       </c>
@@ -3723,7 +3723,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
         <v>24</v>
       </c>
@@ -3739,7 +3739,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
         <v>25</v>
       </c>
@@ -3759,7 +3759,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
         <v>26</v>
       </c>
@@ -3779,7 +3779,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
         <v>27</v>
       </c>
@@ -3799,7 +3799,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" s="1">
         <v>28</v>
       </c>
@@ -3819,7 +3819,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" s="1">
         <v>29</v>
       </c>
@@ -3839,7 +3839,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" s="1">
         <v>30</v>
       </c>
@@ -3859,7 +3859,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" s="1">
         <v>31</v>
       </c>
@@ -3879,7 +3879,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" s="1">
         <v>32</v>
       </c>
@@ -3899,7 +3899,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" s="1">
         <v>33</v>
       </c>
@@ -3919,7 +3919,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" s="1">
         <v>34</v>
       </c>
@@ -3939,7 +3939,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" s="1">
         <v>35</v>
       </c>
@@ -3959,7 +3959,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" s="1">
         <v>36</v>
       </c>
@@ -3979,7 +3979,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" s="1">
         <v>37</v>
       </c>
@@ -3999,7 +3999,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39" s="1">
         <v>38</v>
       </c>
@@ -4019,7 +4019,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40" s="1">
         <v>39</v>
       </c>
@@ -4039,7 +4039,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" s="1">
         <v>40</v>
       </c>
@@ -4059,7 +4059,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" s="1">
         <v>41</v>
       </c>
@@ -4079,7 +4079,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43" s="1">
         <v>42</v>
       </c>
@@ -4099,7 +4099,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44" s="1">
         <v>43</v>
       </c>
@@ -4119,7 +4119,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45" s="1">
         <v>44</v>
       </c>
@@ -4139,7 +4139,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46" s="1">
         <v>45</v>
       </c>
@@ -4159,7 +4159,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47" s="1">
         <v>46</v>
       </c>
@@ -4179,7 +4179,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A48" s="1">
         <v>47</v>
       </c>
@@ -4199,7 +4199,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A49" s="1">
         <v>48</v>
       </c>
@@ -4219,7 +4219,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A50" s="1">
         <v>49</v>
       </c>
@@ -4239,7 +4239,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A51" s="1">
         <v>50</v>
       </c>
@@ -4259,7 +4259,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A52" s="1">
         <v>51</v>
       </c>
@@ -4279,7 +4279,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A53" s="1">
         <v>52</v>
       </c>
@@ -4299,7 +4299,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A54" s="1">
         <v>53</v>
       </c>
@@ -4319,7 +4319,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A55" s="1">
         <v>54</v>
       </c>
@@ -4339,7 +4339,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A56" s="1">
         <v>55</v>
       </c>
@@ -4359,7 +4359,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A57" s="1">
         <v>56</v>
       </c>
@@ -4379,7 +4379,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A58" s="1">
         <v>57</v>
       </c>
@@ -4399,7 +4399,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A59" s="1">
         <v>58</v>
       </c>
@@ -4419,7 +4419,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A60" s="1">
         <v>59</v>
       </c>
@@ -4439,7 +4439,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A61" s="1">
         <v>60</v>
       </c>
@@ -4459,7 +4459,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A62" s="1">
         <v>61</v>
       </c>
@@ -4479,7 +4479,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A63" s="1">
         <v>62</v>
       </c>
@@ -4499,7 +4499,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A64" s="1">
         <v>63</v>
       </c>
@@ -4519,7 +4519,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A65" s="1">
         <v>64</v>
       </c>
@@ -4539,7 +4539,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A66" s="1">
         <v>65</v>
       </c>
@@ -4556,7 +4556,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A67" s="1">
         <v>66</v>
       </c>
@@ -4570,7 +4570,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A68" s="1">
         <v>67</v>
       </c>
@@ -4584,7 +4584,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A69" s="1">
         <v>68</v>
       </c>
@@ -4598,7 +4598,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A70" s="1">
         <v>69</v>
       </c>
@@ -4612,7 +4612,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A71" s="1">
         <v>70</v>
       </c>
@@ -4626,7 +4626,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A72" s="1">
         <v>71</v>
       </c>
@@ -4640,7 +4640,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A73" s="1">
         <v>72</v>
       </c>
@@ -4654,7 +4654,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A74" s="1">
         <v>73</v>
       </c>
@@ -4668,7 +4668,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A75" s="1">
         <v>74</v>
       </c>
@@ -4696,9 +4696,9 @@
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1">
         <v>1</v>
       </c>
@@ -4706,7 +4706,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>2</v>
       </c>
@@ -4714,7 +4714,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>3</v>
       </c>
@@ -4722,7 +4722,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>4</v>
       </c>
@@ -4743,9 +4743,9 @@
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1">
         <v>1</v>
       </c>
@@ -4753,7 +4753,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>2</v>
       </c>
@@ -4761,7 +4761,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>3</v>
       </c>
@@ -4769,7 +4769,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>4</v>
       </c>
@@ -4777,7 +4777,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>5</v>
       </c>
@@ -4788,7 +4788,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>6</v>
       </c>
@@ -4796,7 +4796,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>7</v>
       </c>
@@ -4804,7 +4804,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>8</v>
       </c>
@@ -4812,7 +4812,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>9</v>
       </c>
@@ -4820,7 +4820,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>10</v>
       </c>
@@ -4841,9 +4841,9 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1">
         <v>1</v>
       </c>
@@ -4851,7 +4851,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>2</v>
       </c>
@@ -4859,7 +4859,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>3</v>
       </c>
@@ -4867,7 +4867,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>4</v>
       </c>
@@ -4875,7 +4875,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>5</v>
       </c>
@@ -4883,7 +4883,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>6</v>
       </c>
@@ -4891,7 +4891,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>7</v>
       </c>
@@ -4899,7 +4899,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>8</v>
       </c>
@@ -4907,7 +4907,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>9</v>
       </c>
@@ -4915,7 +4915,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>10</v>
       </c>
@@ -4923,7 +4923,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>11</v>
       </c>
@@ -4931,7 +4931,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>12</v>
       </c>

</xml_diff>

<commit_message>
upd: Introduced sub-cell type 0 for Mix B cell and 1 for Mix T cell
</commit_message>
<xml_diff>
--- a/DesignMatrix.xlsx
+++ b/DesignMatrix.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11110"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27A1861D-61EB-DF40-AF36-C355F6A38205}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE25D358-ABB6-6B45-B493-48D179C45444}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25440" windowHeight="15400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25440" windowHeight="15400" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DesignMatrix" sheetId="2" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="380" uniqueCount="199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="381" uniqueCount="200">
   <si>
     <t>Sample index</t>
   </si>
@@ -162,9 +162,6 @@
     <t>ENCFF442UGX-1.fastq.gz, ENCFF556DET-2.fastq.gz</t>
   </si>
   <si>
-    <t>Mix</t>
-  </si>
-  <si>
     <t>CD8+ T cell</t>
   </si>
   <si>
@@ -628,6 +625,12 @@
   </si>
   <si>
     <t>ENCBS714KQF, ENCFF088DIY</t>
+  </si>
+  <si>
+    <t>Mix B cell</t>
+  </si>
+  <si>
+    <t>Mix T cell</t>
   </si>
 </sst>
 </file>
@@ -988,8 +991,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F369D9C3-2B00-4B3E-B4DE-89D514952C05}">
   <dimension ref="B2:DC10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="BH1" workbookViewId="0">
-      <selection activeCell="CJ16" sqref="CJ16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1010,13 +1013,13 @@
         <v>4</v>
       </c>
       <c r="AB2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="BO2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="BY2" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="3" spans="2:107" x14ac:dyDescent="0.2">
@@ -2464,25 +2467,25 @@
         <v>33</v>
       </c>
       <c r="C8" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D8" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E8" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F8" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G8" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H8" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I8" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J8" s="4">
         <v>2</v>
@@ -2500,22 +2503,22 @@
         <v>2</v>
       </c>
       <c r="O8" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P8" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q8" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R8" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S8" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T8" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U8" s="4">
         <v>1</v>
@@ -2545,10 +2548,10 @@
         <v>2</v>
       </c>
       <c r="AD8" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE8" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AF8" s="4">
         <v>3</v>
@@ -2587,22 +2590,22 @@
         <v>4</v>
       </c>
       <c r="AR8" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AS8" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AT8" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AU8" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AV8" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AW8" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AX8" s="4">
         <v>5</v>
@@ -2623,13 +2626,13 @@
         <v>9</v>
       </c>
       <c r="BD8" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BE8" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BF8" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BG8" s="4">
         <v>5</v>
@@ -2656,19 +2659,19 @@
         <v>12</v>
       </c>
       <c r="BO8" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BP8" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BQ8" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BR8" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BS8" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BT8" s="4">
         <v>1</v>
@@ -2710,28 +2713,28 @@
         <v>1</v>
       </c>
       <c r="CG8" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CH8" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CI8" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CJ8" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CK8" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CL8" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CM8" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CN8" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CO8" s="4">
         <v>1</v>
@@ -2743,31 +2746,31 @@
         <v>1</v>
       </c>
       <c r="CR8" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CS8" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CT8" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CU8" s="4">
         <v>1</v>
       </c>
       <c r="CV8" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CW8" s="4">
         <v>1</v>
       </c>
       <c r="CX8" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CY8" s="4">
         <v>10</v>
       </c>
       <c r="CZ8" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="DA8" s="4">
         <v>2</v>
@@ -2776,12 +2779,12 @@
         <v>1</v>
       </c>
       <c r="DC8" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="2:107" x14ac:dyDescent="0.2">
       <c r="B9" s="3" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C9" s="4">
         <v>1</v>
@@ -3101,7 +3104,7 @@
     </row>
     <row r="10" spans="2:107" x14ac:dyDescent="0.2">
       <c r="B10" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C10" s="4"/>
       <c r="D10" s="4">
@@ -3245,7 +3248,7 @@
         <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
@@ -3253,7 +3256,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
   </sheetData>
@@ -3333,10 +3336,10 @@
         <v>7</v>
       </c>
       <c r="E3" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="F3" s="1" t="s">
         <v>49</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
@@ -3356,7 +3359,7 @@
         <v>36</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
@@ -3376,7 +3379,7 @@
         <v>36</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
@@ -3393,10 +3396,10 @@
         <v>7</v>
       </c>
       <c r="E6" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="F6" s="1" t="s">
         <v>53</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
@@ -3416,7 +3419,7 @@
         <v>36</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
@@ -3436,7 +3439,7 @@
         <v>36</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
@@ -3453,10 +3456,10 @@
         <v>8</v>
       </c>
       <c r="E9" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F9" s="1" t="s">
         <v>46</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
@@ -3473,10 +3476,10 @@
         <v>8</v>
       </c>
       <c r="E10" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="F10" s="1" t="s">
         <v>60</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
@@ -3527,13 +3530,13 @@
         <v>4</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F13" s="1" t="s">
         <v>42</v>
@@ -3747,16 +3750,16 @@
         <v>4</v>
       </c>
       <c r="C26" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D26" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
@@ -3764,19 +3767,19 @@
         <v>26</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D27" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E27" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="F27" s="1" t="s">
         <v>63</v>
-      </c>
-      <c r="F27" s="1" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
@@ -3784,19 +3787,19 @@
         <v>27</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D28" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
@@ -3804,19 +3807,19 @@
         <v>28</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D29" s="1" t="s">
         <v>7</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
@@ -3824,19 +3827,19 @@
         <v>29</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D30" s="1" t="s">
         <v>7</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
@@ -3844,19 +3847,19 @@
         <v>30</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D31" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E31" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="F31" s="1" t="s">
         <v>75</v>
-      </c>
-      <c r="F31" s="1" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
@@ -3864,19 +3867,19 @@
         <v>31</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D32" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.2">
@@ -3884,19 +3887,19 @@
         <v>32</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D33" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.2">
@@ -3904,19 +3907,19 @@
         <v>33</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D34" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.2">
@@ -3924,19 +3927,19 @@
         <v>34</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D35" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
@@ -3944,19 +3947,19 @@
         <v>35</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D36" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">
@@ -3964,19 +3967,19 @@
         <v>36</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D37" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.2">
@@ -3984,19 +3987,19 @@
         <v>37</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D38" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.2">
@@ -4004,19 +4007,19 @@
         <v>38</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D39" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.2">
@@ -4024,19 +4027,19 @@
         <v>39</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D40" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.2">
@@ -4044,19 +4047,19 @@
         <v>40</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D41" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E41" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="F41" s="1" t="s">
         <v>96</v>
-      </c>
-      <c r="F41" s="1" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.2">
@@ -4064,19 +4067,19 @@
         <v>41</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D42" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.2">
@@ -4084,19 +4087,19 @@
         <v>42</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D43" s="1" t="s">
         <v>7</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.2">
@@ -4104,19 +4107,19 @@
         <v>43</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D44" s="1" t="s">
         <v>7</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.2">
@@ -4124,19 +4127,19 @@
         <v>44</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D45" s="1" t="s">
         <v>7</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.2">
@@ -4144,19 +4147,19 @@
         <v>45</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D46" s="1" t="s">
         <v>7</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.2">
@@ -4164,19 +4167,19 @@
         <v>46</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D47" s="1" t="s">
         <v>7</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.2">
@@ -4184,19 +4187,19 @@
         <v>47</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D48" s="1" t="s">
         <v>7</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.2">
@@ -4204,19 +4207,19 @@
         <v>48</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D49" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.2">
@@ -4224,19 +4227,19 @@
         <v>49</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D50" s="1" t="s">
         <v>7</v>
       </c>
       <c r="E50" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="F50" s="1" t="s">
         <v>122</v>
-      </c>
-      <c r="F50" s="1" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.2">
@@ -4244,19 +4247,19 @@
         <v>50</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D51" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F51" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.2">
@@ -4264,19 +4267,19 @@
         <v>51</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D52" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.2">
@@ -4284,19 +4287,19 @@
         <v>52</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D53" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E53" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="F53" s="1" t="s">
         <v>132</v>
-      </c>
-      <c r="F53" s="1" t="s">
-        <v>133</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.2">
@@ -4304,19 +4307,19 @@
         <v>53</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D54" s="1" t="s">
         <v>7</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F54" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.2">
@@ -4324,19 +4327,19 @@
         <v>54</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D55" s="1" t="s">
         <v>7</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="F55" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.2">
@@ -4344,19 +4347,19 @@
         <v>55</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D56" s="1" t="s">
         <v>7</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="F56" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.2">
@@ -4364,19 +4367,19 @@
         <v>56</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D57" s="1" t="s">
         <v>7</v>
       </c>
       <c r="E57" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="F57" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.2">
@@ -4384,19 +4387,19 @@
         <v>57</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D58" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="F58" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.2">
@@ -4404,19 +4407,19 @@
         <v>58</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D59" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="F59" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.2">
@@ -4424,19 +4427,19 @@
         <v>59</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D60" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="F60" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.2">
@@ -4444,19 +4447,19 @@
         <v>60</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C61" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D61" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="F61" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.2">
@@ -4464,19 +4467,19 @@
         <v>61</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C62" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D62" s="1" t="s">
         <v>7</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="F62" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.2">
@@ -4484,19 +4487,19 @@
         <v>62</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C63" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D63" s="1" t="s">
         <v>7</v>
       </c>
       <c r="E63" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="F63" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.2">
@@ -4504,19 +4507,19 @@
         <v>63</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C64" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D64" s="1" t="s">
         <v>7</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="F64" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.2">
@@ -4524,19 +4527,19 @@
         <v>64</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C65" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D65" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E65" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="F65" s="1" t="s">
         <v>166</v>
-      </c>
-      <c r="F65" s="1" t="s">
-        <v>167</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.2">
@@ -4544,16 +4547,16 @@
         <v>65</v>
       </c>
       <c r="B66" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="C66" t="s">
         <v>169</v>
-      </c>
-      <c r="C66" t="s">
-        <v>170</v>
       </c>
       <c r="D66" s="1" t="s">
         <v>7</v>
       </c>
       <c r="E66" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.2">
@@ -4561,10 +4564,10 @@
         <v>66</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C67" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D67" s="1" t="s">
         <v>7</v>
@@ -4575,10 +4578,10 @@
         <v>67</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C68" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D68" s="1" t="s">
         <v>7</v>
@@ -4589,10 +4592,10 @@
         <v>68</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C69" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D69" s="1" t="s">
         <v>7</v>
@@ -4603,10 +4606,10 @@
         <v>69</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C70" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D70" s="1" t="s">
         <v>7</v>
@@ -4617,10 +4620,10 @@
         <v>70</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C71" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D71" s="1" t="s">
         <v>8</v>
@@ -4631,10 +4634,10 @@
         <v>71</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C72" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D72" s="1" t="s">
         <v>8</v>
@@ -4645,10 +4648,10 @@
         <v>72</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C73" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D73" s="1" t="s">
         <v>8</v>
@@ -4659,10 +4662,10 @@
         <v>73</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C74" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D74" s="1" t="s">
         <v>8</v>
@@ -4673,10 +4676,10 @@
         <v>74</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C75" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D75" s="1" t="s">
         <v>8</v>
@@ -4703,7 +4706,7 @@
         <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
@@ -4711,7 +4714,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -4719,7 +4722,7 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
@@ -4727,7 +4730,7 @@
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
   </sheetData>
@@ -4750,7 +4753,7 @@
         <v>1</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
@@ -4758,7 +4761,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -4766,7 +4769,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -4774,7 +4777,7 @@
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
@@ -4782,10 +4785,10 @@
         <v>5</v>
       </c>
       <c r="B5" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="C5" t="s">
         <v>68</v>
-      </c>
-      <c r="C5" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
@@ -4793,7 +4796,7 @@
         <v>6</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
@@ -4801,7 +4804,7 @@
         <v>7</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
@@ -4809,7 +4812,7 @@
         <v>8</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
@@ -4817,7 +4820,7 @@
         <v>9</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
@@ -4825,7 +4828,7 @@
         <v>10</v>
       </c>
       <c r="B10" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
   </sheetData>
@@ -4835,9 +4838,9 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6499CB2B-6832-4092-A9EA-DD66A17F48BA}">
-  <dimension ref="A1:B12"/>
+  <dimension ref="A1:B13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -4845,98 +4848,106 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>43</v>
+        <v>198</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>44</v>
+        <v>199</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>70</v>
+        <v>43</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>101</v>
+        <v>69</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>120</v>
+        <v>100</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>156</v>
+        <v>137</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13">
         <v>12</v>
       </c>
-      <c r="B12" t="s">
-        <v>168</v>
+      <c r="B13" t="s">
+        <v>167</v>
       </c>
     </row>
   </sheetData>

</xml_diff>